<commit_message>
model and statistics fixes
</commit_message>
<xml_diff>
--- a/output/LUAD_statistics_all subtypes.xlsx
+++ b/output/LUAD_statistics_all subtypes.xlsx
@@ -63,51 +63,51 @@
     <t>7</t>
   </si>
   <si>
+    <t>9</t>
+  </si>
+  <si>
     <t>36</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
     <t>29</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>6</t>
   </si>
   <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
     <t>15</t>
   </si>
   <si>
     <t>17</t>
   </si>
   <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>19</t>
   </si>
   <si>
     <t>31</t>
   </si>
   <si>
-    <t>32</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -225,36 +225,36 @@
     <t>Mutation KRAS</t>
   </si>
   <si>
+    <t>Amplification CDK4</t>
+  </si>
+  <si>
     <t>Pattern OR_KRAS</t>
   </si>
   <si>
-    <t>Amplification CDK4</t>
-  </si>
-  <si>
     <t>Mutation TP53</t>
   </si>
   <si>
+    <t>Mutation ATM</t>
+  </si>
+  <si>
     <t>Pattern OR_CDK4_TP53</t>
   </si>
   <si>
+    <t>Pattern OR_EGFR_SMARCA4</t>
+  </si>
+  <si>
+    <t>Mutation SMARCA4</t>
+  </si>
+  <si>
+    <t>Mutation ARID1B</t>
+  </si>
+  <si>
+    <t>Mutation KEAP1</t>
+  </si>
+  <si>
     <t>Mutation NF1</t>
   </si>
   <si>
-    <t>Mutation SMARCA4</t>
-  </si>
-  <si>
-    <t>Mutation KEAP1</t>
-  </si>
-  <si>
-    <t>Mutation ATM</t>
-  </si>
-  <si>
-    <t>Pattern OR_EGFR_SMARCA4</t>
-  </si>
-  <si>
-    <t>Mutation ARID1B</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -267,31 +267,31 @@
     <t>Amplification KRAS</t>
   </si>
   <si>
+    <t>Amplification MDM2</t>
+  </si>
+  <si>
     <t>Mutation STK11</t>
   </si>
   <si>
-    <t>Amplification MDM2</t>
-  </si>
-  <si>
     <t>Mutation RB1</t>
   </si>
   <si>
+    <t>Deletion CDKN2A</t>
+  </si>
+  <si>
     <t>Mutation NFE2L2</t>
   </si>
   <si>
+    <t>Mutation ROS1</t>
+  </si>
+  <si>
     <t>Amplification MET</t>
   </si>
   <si>
-    <t>Deletion CDKN2A</t>
-  </si>
-  <si>
     <t>Mutation CDKN2A</t>
   </si>
   <si>
     <t>Mutation RET</t>
-  </si>
-  <si>
-    <t>Mutation ROS1</t>
   </si>
   <si>
     <t>Amplification CCNE1</t>
@@ -646,7 +646,7 @@
         <v>0.0591966173361522</v>
       </c>
       <c r="N3" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="4">
@@ -704,19 +704,19 @@
         <v>84</v>
       </c>
       <c r="D5" t="n">
-        <v>158.0</v>
+        <v>29.0</v>
       </c>
       <c r="E5" t="n">
-        <v>84.0</v>
+        <v>26.0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.0177894166197971</v>
       </c>
       <c r="G5" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H5" t="n">
-        <v>1.11208450607907E-5</v>
+        <v>3.80945122355267E-7</v>
       </c>
       <c r="I5" t="n">
         <v>80.0</v>
@@ -725,16 +725,16 @@
         <v>100.0</v>
       </c>
       <c r="K5" t="n">
-        <v>0.17801268498942918</v>
+        <v>0.05496828752642706</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0013371152897117859</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M5" t="n">
-        <v>0.177589852008457</v>
+        <v>0.0549682875264271</v>
       </c>
       <c r="N5" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="6">
@@ -748,37 +748,37 @@
         <v>85</v>
       </c>
       <c r="D6" t="n">
-        <v>29.0</v>
+        <v>158.0</v>
       </c>
       <c r="E6" t="n">
-        <v>26.0</v>
+        <v>84.0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0177894166197971</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G6" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H6" t="n">
-        <v>3.80945122355267E-7</v>
+        <v>1.11208450607907E-5</v>
       </c>
       <c r="I6" t="n">
-        <v>60.0</v>
+        <v>80.0</v>
       </c>
       <c r="J6" t="n">
         <v>100.0</v>
       </c>
       <c r="K6" t="n">
-        <v>0.05496828752642706</v>
+        <v>0.17758985200845667</v>
       </c>
       <c r="L6" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M6" t="n">
-        <v>0.0551797040169133</v>
+        <v>0.177589852008457</v>
       </c>
       <c r="N6" t="n">
-        <v>6.68557644855895E-4</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7">
@@ -816,13 +816,13 @@
         <v>0.06553911205073996</v>
       </c>
       <c r="L7" t="n">
-        <v>6.542051911182396E-18</v>
+        <v>4.625929269271485E-18</v>
       </c>
       <c r="M7" t="n">
         <v>0.06553911205074</v>
       </c>
       <c r="N7" t="n">
-        <v>0.0</v>
+        <v>4.62592926927149E-18</v>
       </c>
     </row>
     <row r="8">
@@ -833,22 +833,22 @@
         <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D8" t="n">
-        <v>265.0</v>
+        <v>46.0</v>
       </c>
       <c r="E8" t="n">
-        <v>28.0</v>
+        <v>19.0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.0058336561716597</v>
       </c>
       <c r="G8" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H8" t="n">
-        <v>1.77721953788421E-6</v>
+        <v>0.00699258708471991</v>
       </c>
       <c r="I8" t="n">
         <v>40.0</v>
@@ -857,16 +857,16 @@
         <v>100.0</v>
       </c>
       <c r="K8" t="n">
-        <v>0.05919661733615222</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="L8" t="n">
         <v>0.0</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0591966173361522</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="N8" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="9">
@@ -877,22 +877,22 @@
         <v>74</v>
       </c>
       <c r="C9" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D9" t="n">
-        <v>64.0</v>
+        <v>265.0</v>
       </c>
       <c r="E9" t="n">
-        <v>25.0</v>
+        <v>28.0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0158730158730159</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0103051123549064</v>
+        <v>1.77721953788421E-6</v>
       </c>
       <c r="I9" t="n">
         <v>40.0</v>
@@ -901,13 +901,13 @@
         <v>100.0</v>
       </c>
       <c r="K9" t="n">
-        <v>0.052854122621564484</v>
+        <v>0.05919661733615222</v>
       </c>
       <c r="L9" t="n">
         <v>0.0</v>
       </c>
       <c r="M9" t="n">
-        <v>0.0528541226215645</v>
+        <v>0.0591966173361522</v>
       </c>
       <c r="N9" t="n">
         <v>0.0</v>
@@ -918,25 +918,25 @@
         <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D10" t="n">
-        <v>158.0</v>
+        <v>265.0</v>
       </c>
       <c r="E10" t="n">
-        <v>46.0</v>
+        <v>34.0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0058336561716597</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G10" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H10" t="n">
-        <v>0.00131454955057744</v>
+        <v>8.27584277446678E-5</v>
       </c>
       <c r="I10" t="n">
         <v>40.0</v>
@@ -945,13 +945,13 @@
         <v>100.0</v>
       </c>
       <c r="K10" t="n">
-        <v>0.09725158562367865</v>
+        <v>0.07188160676532769</v>
       </c>
       <c r="L10" t="n">
         <v>0.0</v>
       </c>
       <c r="M10" t="n">
-        <v>0.0972515856236787</v>
+        <v>0.0718816067653277</v>
       </c>
       <c r="N10" t="n">
         <v>0.0</v>
@@ -968,19 +968,19 @@
         <v>87</v>
       </c>
       <c r="D11" t="n">
-        <v>48.0</v>
+        <v>120.0</v>
       </c>
       <c r="E11" t="n">
-        <v>15.0</v>
+        <v>82.0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0058336561716597</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G11" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H11" t="n">
-        <v>0.00161509241969472</v>
+        <v>4.12608987825272E-4</v>
       </c>
       <c r="I11" t="n">
         <v>40.0</v>
@@ -989,13 +989,13 @@
         <v>100.0</v>
       </c>
       <c r="K11" t="n">
-        <v>0.03171247357293869</v>
+        <v>0.1733615221987315</v>
       </c>
       <c r="L11" t="n">
         <v>0.0</v>
       </c>
       <c r="M11" t="n">
-        <v>0.0317124735729387</v>
+        <v>0.173361522198731</v>
       </c>
       <c r="N11" t="n">
         <v>0.0</v>
@@ -1009,22 +1009,22 @@
         <v>76</v>
       </c>
       <c r="C12" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D12" t="n">
-        <v>93.0</v>
+        <v>48.0</v>
       </c>
       <c r="E12" t="n">
-        <v>84.0</v>
+        <v>15.0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.200982679178368</v>
+        <v>0.0058336561716597</v>
       </c>
       <c r="G12" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H12" t="n">
-        <v>3.59155834889592E-4</v>
+        <v>0.00161509241969472</v>
       </c>
       <c r="I12" t="n">
         <v>40.0</v>
@@ -1033,13 +1033,13 @@
         <v>100.0</v>
       </c>
       <c r="K12" t="n">
-        <v>0.17801268498942918</v>
+        <v>0.03171247357293869</v>
       </c>
       <c r="L12" t="n">
-        <v>0.0013371152897117859</v>
+        <v>0.0</v>
       </c>
       <c r="M12" t="n">
-        <v>0.177589852008457</v>
+        <v>0.0317124735729387</v>
       </c>
       <c r="N12" t="n">
         <v>0.0</v>
@@ -1050,40 +1050,40 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D13" t="n">
-        <v>265.0</v>
+        <v>25.0</v>
       </c>
       <c r="E13" t="n">
-        <v>34.0</v>
+        <v>26.0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.414406187123225</v>
       </c>
       <c r="G13" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H13" t="n">
-        <v>8.27584277446678E-5</v>
+        <v>0.00877923124276454</v>
       </c>
       <c r="I13" t="n">
-        <v>20.0</v>
+        <v>40.0</v>
       </c>
       <c r="J13" t="n">
         <v>100.0</v>
       </c>
       <c r="K13" t="n">
-        <v>0.07188160676532769</v>
+        <v>0.05496828752642706</v>
       </c>
       <c r="L13" t="n">
         <v>0.0</v>
       </c>
       <c r="M13" t="n">
-        <v>0.0718816067653277</v>
+        <v>0.0549682875264271</v>
       </c>
       <c r="N13" t="n">
         <v>0.0</v>
@@ -1094,40 +1094,40 @@
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C14" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D14" t="n">
-        <v>103.0</v>
+        <v>93.0</v>
       </c>
       <c r="E14" t="n">
-        <v>15.0</v>
+        <v>84.0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.200982679178368</v>
       </c>
       <c r="G14" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H14" t="n">
-        <v>0.00167276266869532</v>
+        <v>3.59155834889592E-4</v>
       </c>
       <c r="I14" t="n">
-        <v>20.0</v>
+        <v>40.0</v>
       </c>
       <c r="J14" t="n">
         <v>100.0</v>
       </c>
       <c r="K14" t="n">
-        <v>0.03171247357293869</v>
+        <v>0.17758985200845667</v>
       </c>
       <c r="L14" t="n">
         <v>0.0</v>
       </c>
       <c r="M14" t="n">
-        <v>0.0317124735729387</v>
+        <v>0.177589852008457</v>
       </c>
       <c r="N14" t="n">
         <v>0.0</v>
@@ -1138,40 +1138,40 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" t="s">
         <v>77</v>
       </c>
-      <c r="C15" t="s">
-        <v>81</v>
-      </c>
       <c r="D15" t="n">
-        <v>46.0</v>
+        <v>64.0</v>
       </c>
       <c r="E15" t="n">
-        <v>19.0</v>
+        <v>25.0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0058336561716597</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G15" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0158730158730159</v>
       </c>
       <c r="H15" t="n">
-        <v>0.00699258708471991</v>
+        <v>0.0103051123549064</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="J15" t="n">
         <v>100.0</v>
       </c>
       <c r="K15" t="n">
-        <v>0.040169133192389</v>
+        <v>0.052854122621564484</v>
       </c>
       <c r="L15" t="n">
-        <v>0.0</v>
+        <v>3.271025955591198E-18</v>
       </c>
       <c r="M15" t="n">
-        <v>0.040169133192389</v>
+        <v>0.0528541226215645</v>
       </c>
       <c r="N15" t="n">
         <v>0.0</v>
@@ -1182,40 +1182,40 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="D16" t="n">
-        <v>120.0</v>
+        <v>158.0</v>
       </c>
       <c r="E16" t="n">
-        <v>82.0</v>
+        <v>46.0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0058336561716597</v>
       </c>
       <c r="G16" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H16" t="n">
-        <v>4.12608987825272E-4</v>
+        <v>0.00131454955057744</v>
       </c>
       <c r="I16" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="J16" t="n">
         <v>100.0</v>
       </c>
       <c r="K16" t="n">
-        <v>0.1733615221987315</v>
+        <v>0.09725158562367865</v>
       </c>
       <c r="L16" t="n">
         <v>0.0</v>
       </c>
       <c r="M16" t="n">
-        <v>0.173361522198731</v>
+        <v>0.0972515856236787</v>
       </c>
       <c r="N16" t="n">
         <v>0.0</v>
@@ -1226,16 +1226,16 @@
         <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C17" t="s">
         <v>90</v>
       </c>
       <c r="D17" t="n">
-        <v>250.0</v>
+        <v>103.0</v>
       </c>
       <c r="E17" t="n">
-        <v>25.0</v>
+        <v>15.0</v>
       </c>
       <c r="F17" t="n">
         <v>0.00396825396825397</v>
@@ -1244,7 +1244,7 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H17" t="n">
-        <v>0.00148405904181779</v>
+        <v>0.00167276266869532</v>
       </c>
       <c r="I17" t="n">
         <v>0.0</v>
@@ -1253,13 +1253,13 @@
         <v>100.0</v>
       </c>
       <c r="K17" t="n">
-        <v>0.052854122621564484</v>
+        <v>0.03171247357293869</v>
       </c>
       <c r="L17" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M17" t="n">
-        <v>0.0528541226215645</v>
+        <v>0.0317124735729387</v>
       </c>
       <c r="N17" t="n">
         <v>0.0</v>
@@ -1270,16 +1270,16 @@
         <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" t="s">
         <v>91</v>
       </c>
       <c r="D18" t="n">
-        <v>265.0</v>
+        <v>250.0</v>
       </c>
       <c r="E18" t="n">
-        <v>23.0</v>
+        <v>25.0</v>
       </c>
       <c r="F18" t="n">
         <v>0.00396825396825397</v>
@@ -1288,7 +1288,7 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H18" t="n">
-        <v>9.13202144083936E-5</v>
+        <v>0.00148405904181779</v>
       </c>
       <c r="I18" t="n">
         <v>0.0</v>
@@ -1297,13 +1297,13 @@
         <v>100.0</v>
       </c>
       <c r="K18" t="n">
-        <v>0.048625792811839326</v>
+        <v>0.052854122621564484</v>
       </c>
       <c r="L18" t="n">
         <v>0.0</v>
       </c>
       <c r="M18" t="n">
-        <v>0.0486257928118393</v>
+        <v>0.0528541226215645</v>
       </c>
       <c r="N18" t="n">
         <v>0.0</v>
@@ -1314,25 +1314,25 @@
         <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C19" t="s">
         <v>92</v>
       </c>
       <c r="D19" t="n">
-        <v>25.0</v>
+        <v>265.0</v>
       </c>
       <c r="E19" t="n">
-        <v>26.0</v>
+        <v>23.0</v>
       </c>
       <c r="F19" t="n">
-        <v>0.414406187123225</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G19" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H19" t="n">
-        <v>0.00877923124276454</v>
+        <v>9.13202144083936E-5</v>
       </c>
       <c r="I19" t="n">
         <v>0.0</v>
@@ -1341,13 +1341,13 @@
         <v>100.0</v>
       </c>
       <c r="K19" t="n">
-        <v>0.05496828752642706</v>
+        <v>0.048625792811839326</v>
       </c>
       <c r="L19" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M19" t="n">
-        <v>0.0549682875264271</v>
+        <v>0.0486257928118393</v>
       </c>
       <c r="N19" t="n">
         <v>2.31296463463574E-18</v>
@@ -1405,7 +1405,7 @@
         <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D21" t="e">
         <v>#NUM!</v>
@@ -1432,7 +1432,7 @@
         <v>0.0613107822410148</v>
       </c>
       <c r="L21" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M21" t="e">
         <v>#NUM!</v>
@@ -1757,7 +1757,7 @@
         <v>80</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D29" t="e">
         <v>#NUM!</v>
@@ -1916,7 +1916,7 @@
         <v>0.06553911205073996</v>
       </c>
       <c r="L32" t="n">
-        <v>4.625929269271485E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M32" t="e">
         <v>#NUM!</v>
@@ -1933,7 +1933,7 @@
         <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D33" t="e">
         <v>#NUM!</v>
@@ -2109,7 +2109,7 @@
         <v>80</v>
       </c>
       <c r="C37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D37" t="e">
         <v>#NUM!</v>
@@ -2285,7 +2285,7 @@
         <v>80</v>
       </c>
       <c r="C41" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D41" t="e">
         <v>#NUM!</v>
@@ -2441,10 +2441,10 @@
         <v>#NUM!</v>
       </c>
       <c r="K44" t="n">
-        <v>0.4885835095137421</v>
+        <v>0.48710359408033826</v>
       </c>
       <c r="L44" t="n">
-        <v>0.011382945174485744</v>
+        <v>0.009359807027982536</v>
       </c>
       <c r="M44" t="e">
         <v>#NUM!</v>
@@ -2505,7 +2505,7 @@
         <v>80</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D46" t="e">
         <v>#NUM!</v>
@@ -2593,7 +2593,7 @@
         <v>80</v>
       </c>
       <c r="C48" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D48" t="e">
         <v>#NUM!</v>
@@ -3038,7 +3038,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>68</v>
@@ -3074,15 +3074,15 @@
         <v>0.0</v>
       </c>
       <c r="M3" t="n">
-        <v>0.122198731501057</v>
+        <v>0.126427061310782</v>
       </c>
       <c r="N3" t="n">
-        <v>0.00674474199521094</v>
+        <v>0.00579416625541775</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>69</v>
@@ -3126,7 +3126,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
         <v>70</v>
@@ -3135,19 +3135,19 @@
         <v>84</v>
       </c>
       <c r="D5" t="n">
-        <v>158.0</v>
+        <v>29.0</v>
       </c>
       <c r="E5" t="n">
-        <v>84.0</v>
+        <v>26.0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.0177894166197971</v>
       </c>
       <c r="G5" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H5" t="n">
-        <v>1.11208450607907E-5</v>
+        <v>3.80945122355267E-7</v>
       </c>
       <c r="I5" t="n">
         <v>80.0</v>
@@ -3156,21 +3156,21 @@
         <v>100.0</v>
       </c>
       <c r="K5" t="n">
-        <v>0.17801268498942918</v>
+        <v>0.05496828752642706</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0013371152897117859</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M5" t="n">
-        <v>0.177589852008457</v>
+        <v>0.0558139534883721</v>
       </c>
       <c r="N5" t="n">
-        <v>0.0</v>
+        <v>0.00267423057942358</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>131</v>
       </c>
       <c r="B6" t="s">
         <v>71</v>
@@ -3179,34 +3179,34 @@
         <v>85</v>
       </c>
       <c r="D6" t="n">
-        <v>29.0</v>
+        <v>158.0</v>
       </c>
       <c r="E6" t="n">
-        <v>26.0</v>
+        <v>84.0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0177894166197971</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G6" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H6" t="n">
-        <v>3.80945122355267E-7</v>
+        <v>1.11208450607907E-5</v>
       </c>
       <c r="I6" t="n">
-        <v>60.0</v>
+        <v>80.0</v>
       </c>
       <c r="J6" t="n">
         <v>100.0</v>
       </c>
       <c r="K6" t="n">
-        <v>0.05496828752642706</v>
+        <v>0.17758985200845667</v>
       </c>
       <c r="L6" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M6" t="n">
-        <v>0.0549682875264271</v>
+        <v>0.177589852008457</v>
       </c>
       <c r="N6" t="n">
         <v>0.0</v>
@@ -3247,39 +3247,39 @@
         <v>0.06553911205073996</v>
       </c>
       <c r="L7" t="n">
-        <v>6.542051911182396E-18</v>
+        <v>4.625929269271485E-18</v>
       </c>
       <c r="M7" t="n">
         <v>0.06553911205074</v>
       </c>
       <c r="N7" t="n">
-        <v>4.62592926927149E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D8" t="n">
-        <v>265.0</v>
+        <v>46.0</v>
       </c>
       <c r="E8" t="n">
-        <v>28.0</v>
+        <v>19.0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.0058336561716597</v>
       </c>
       <c r="G8" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H8" t="n">
-        <v>1.77721953788421E-6</v>
+        <v>0.00699258708471991</v>
       </c>
       <c r="I8" t="n">
         <v>40.0</v>
@@ -3288,42 +3288,42 @@
         <v>100.0</v>
       </c>
       <c r="K8" t="n">
-        <v>0.05919661733615222</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="L8" t="n">
         <v>0.0</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0600422832980973</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="N8" t="n">
-        <v>0.00267423057942358</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
         <v>74</v>
       </c>
       <c r="C9" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D9" t="n">
-        <v>64.0</v>
+        <v>265.0</v>
       </c>
       <c r="E9" t="n">
-        <v>25.0</v>
+        <v>28.0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0158730158730159</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0103051123549064</v>
+        <v>1.77721953788421E-6</v>
       </c>
       <c r="I9" t="n">
         <v>40.0</v>
@@ -3332,42 +3332,42 @@
         <v>100.0</v>
       </c>
       <c r="K9" t="n">
-        <v>0.052854122621564484</v>
+        <v>0.05919661733615222</v>
       </c>
       <c r="L9" t="n">
         <v>0.0</v>
       </c>
       <c r="M9" t="n">
-        <v>0.0528541226215645</v>
+        <v>0.0591966173361522</v>
       </c>
       <c r="N9" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D10" t="n">
-        <v>158.0</v>
+        <v>265.0</v>
       </c>
       <c r="E10" t="n">
-        <v>46.0</v>
+        <v>34.0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0058336561716597</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G10" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H10" t="n">
-        <v>0.00131454955057744</v>
+        <v>8.27584277446678E-5</v>
       </c>
       <c r="I10" t="n">
         <v>40.0</v>
@@ -3376,13 +3376,13 @@
         <v>100.0</v>
       </c>
       <c r="K10" t="n">
-        <v>0.09725158562367865</v>
+        <v>0.07188160676532769</v>
       </c>
       <c r="L10" t="n">
         <v>0.0</v>
       </c>
       <c r="M10" t="n">
-        <v>0.0972515856236787</v>
+        <v>0.0718816067653277</v>
       </c>
       <c r="N10" t="n">
         <v>0.0</v>
@@ -3390,7 +3390,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
         <v>75</v>
@@ -3399,19 +3399,19 @@
         <v>87</v>
       </c>
       <c r="D11" t="n">
-        <v>48.0</v>
+        <v>120.0</v>
       </c>
       <c r="E11" t="n">
-        <v>15.0</v>
+        <v>82.0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0058336561716597</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G11" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H11" t="n">
-        <v>0.00161509241969472</v>
+        <v>4.12608987825272E-4</v>
       </c>
       <c r="I11" t="n">
         <v>40.0</v>
@@ -3420,13 +3420,13 @@
         <v>100.0</v>
       </c>
       <c r="K11" t="n">
-        <v>0.03171247357293869</v>
+        <v>0.1733615221987315</v>
       </c>
       <c r="L11" t="n">
         <v>0.0</v>
       </c>
       <c r="M11" t="n">
-        <v>0.0317124735729387</v>
+        <v>0.173361522198731</v>
       </c>
       <c r="N11" t="n">
         <v>0.0</v>
@@ -3434,28 +3434,28 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
         <v>76</v>
       </c>
       <c r="C12" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D12" t="n">
-        <v>93.0</v>
+        <v>48.0</v>
       </c>
       <c r="E12" t="n">
-        <v>84.0</v>
+        <v>15.0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.200982679178368</v>
+        <v>0.0058336561716597</v>
       </c>
       <c r="G12" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H12" t="n">
-        <v>3.59155834889592E-4</v>
+        <v>0.00161509241969472</v>
       </c>
       <c r="I12" t="n">
         <v>40.0</v>
@@ -3464,13 +3464,13 @@
         <v>100.0</v>
       </c>
       <c r="K12" t="n">
-        <v>0.17801268498942918</v>
+        <v>0.03171247357293869</v>
       </c>
       <c r="L12" t="n">
-        <v>0.0013371152897117859</v>
+        <v>0.0</v>
       </c>
       <c r="M12" t="n">
-        <v>0.177589852008457</v>
+        <v>0.0317124735729387</v>
       </c>
       <c r="N12" t="n">
         <v>0.0</v>
@@ -3478,87 +3478,87 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D13" t="n">
-        <v>265.0</v>
+        <v>25.0</v>
       </c>
       <c r="E13" t="n">
-        <v>34.0</v>
+        <v>26.0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.414406187123225</v>
       </c>
       <c r="G13" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H13" t="n">
-        <v>8.27584277446678E-5</v>
+        <v>0.00877923124276454</v>
       </c>
       <c r="I13" t="n">
-        <v>20.0</v>
+        <v>40.0</v>
       </c>
       <c r="J13" t="n">
         <v>100.0</v>
       </c>
       <c r="K13" t="n">
-        <v>0.07188160676532769</v>
+        <v>0.05496828752642706</v>
       </c>
       <c r="L13" t="n">
         <v>0.0</v>
       </c>
       <c r="M13" t="n">
-        <v>0.0718816067653277</v>
+        <v>0.0551797040169133</v>
       </c>
       <c r="N13" t="n">
-        <v>0.0</v>
+        <v>6.68557644855895E-4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>132</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C14" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D14" t="n">
-        <v>103.0</v>
+        <v>93.0</v>
       </c>
       <c r="E14" t="n">
-        <v>15.0</v>
+        <v>84.0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.200982679178368</v>
       </c>
       <c r="G14" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H14" t="n">
-        <v>0.00167276266869532</v>
+        <v>3.59155834889592E-4</v>
       </c>
       <c r="I14" t="n">
-        <v>20.0</v>
+        <v>40.0</v>
       </c>
       <c r="J14" t="n">
         <v>100.0</v>
       </c>
       <c r="K14" t="n">
-        <v>0.03171247357293869</v>
+        <v>0.17758985200845667</v>
       </c>
       <c r="L14" t="n">
         <v>0.0</v>
       </c>
       <c r="M14" t="n">
-        <v>0.0317124735729387</v>
+        <v>0.177589852008457</v>
       </c>
       <c r="N14" t="n">
         <v>0.0</v>
@@ -3566,43 +3566,43 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" t="s">
         <v>77</v>
       </c>
-      <c r="C15" t="s">
-        <v>81</v>
-      </c>
       <c r="D15" t="n">
-        <v>46.0</v>
+        <v>64.0</v>
       </c>
       <c r="E15" t="n">
-        <v>19.0</v>
+        <v>25.0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0058336561716597</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G15" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0158730158730159</v>
       </c>
       <c r="H15" t="n">
-        <v>0.00699258708471991</v>
+        <v>0.0103051123549064</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="J15" t="n">
         <v>100.0</v>
       </c>
       <c r="K15" t="n">
-        <v>0.040169133192389</v>
+        <v>0.052854122621564484</v>
       </c>
       <c r="L15" t="n">
-        <v>0.0</v>
+        <v>3.271025955591198E-18</v>
       </c>
       <c r="M15" t="n">
-        <v>0.040169133192389</v>
+        <v>0.0528541226215645</v>
       </c>
       <c r="N15" t="n">
         <v>0.0</v>
@@ -3610,43 +3610,43 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D16" t="n">
-        <v>48.0</v>
+        <v>158.0</v>
       </c>
       <c r="E16" t="n">
-        <v>19.0</v>
+        <v>46.0</v>
       </c>
       <c r="F16" t="n">
         <v>0.0058336561716597</v>
       </c>
       <c r="G16" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="H16" t="n">
-        <v>2.75013925583083E-4</v>
+        <v>0.00131454955057744</v>
       </c>
       <c r="I16" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="J16" t="n">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
       <c r="K16" t="n">
-        <v>0.040169133192389</v>
+        <v>0.09725158562367865</v>
       </c>
       <c r="L16" t="n">
         <v>0.0</v>
       </c>
       <c r="M16" t="n">
-        <v>0.040169133192389</v>
+        <v>0.0972515856236787</v>
       </c>
       <c r="N16" t="n">
         <v>0.0</v>
@@ -3654,28 +3654,28 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C17" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="D17" t="n">
-        <v>250.0</v>
+        <v>48.0</v>
       </c>
       <c r="E17" t="n">
-        <v>27.0</v>
+        <v>19.0</v>
       </c>
       <c r="F17" t="n">
+        <v>0.0058336561716597</v>
+      </c>
+      <c r="G17" t="n">
         <v>0.0059626167965088</v>
       </c>
-      <c r="G17" t="n">
-        <v>0.00396825396825397</v>
-      </c>
       <c r="H17" t="n">
-        <v>0.00580706674183575</v>
+        <v>2.75013925583083E-4</v>
       </c>
       <c r="I17" t="n">
         <v>0.0</v>
@@ -3684,33 +3684,33 @@
         <v>0.0</v>
       </c>
       <c r="K17" t="n">
-        <v>0.05708245243128964</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="L17" t="n">
         <v>0.0</v>
       </c>
       <c r="M17" t="n">
-        <v>0.0570824524312896</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="N17" t="n">
-        <v>3.2710259555912E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="C18" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="D18" t="n">
-        <v>266.0</v>
+        <v>250.0</v>
       </c>
       <c r="E18" t="n">
-        <v>28.0</v>
+        <v>27.0</v>
       </c>
       <c r="F18" t="n">
         <v>0.0059626167965088</v>
@@ -3719,7 +3719,7 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H18" t="n">
-        <v>2.7663019432251E-5</v>
+        <v>0.00580706674183575</v>
       </c>
       <c r="I18" t="n">
         <v>0.0</v>
@@ -3728,13 +3728,13 @@
         <v>0.0</v>
       </c>
       <c r="K18" t="n">
-        <v>0.05919661733615222</v>
+        <v>0.05708245243128964</v>
       </c>
       <c r="L18" t="n">
         <v>0.0</v>
       </c>
       <c r="M18" t="n">
-        <v>0.0591966173361522</v>
+        <v>0.0570824524312896</v>
       </c>
       <c r="N18" t="n">
         <v>0.0</v>
@@ -3742,19 +3742,19 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="C19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D19" t="n">
-        <v>250.0</v>
+        <v>266.0</v>
       </c>
       <c r="E19" t="n">
-        <v>34.0</v>
+        <v>28.0</v>
       </c>
       <c r="F19" t="n">
         <v>0.0059626167965088</v>
@@ -3763,7 +3763,7 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H19" t="n">
-        <v>0.0203099057522167</v>
+        <v>2.7663019432251E-5</v>
       </c>
       <c r="I19" t="n">
         <v>0.0</v>
@@ -3772,33 +3772,33 @@
         <v>0.0</v>
       </c>
       <c r="K19" t="n">
-        <v>0.07188160676532769</v>
+        <v>0.05919661733615222</v>
       </c>
       <c r="L19" t="n">
         <v>0.0</v>
       </c>
       <c r="M19" t="n">
-        <v>0.0718816067653277</v>
+        <v>0.0591966173361522</v>
       </c>
       <c r="N19" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="C20" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D20" t="n">
-        <v>27.0</v>
+        <v>250.0</v>
       </c>
       <c r="E20" t="n">
-        <v>15.0</v>
+        <v>34.0</v>
       </c>
       <c r="F20" t="n">
         <v>0.0059626167965088</v>
@@ -3807,7 +3807,7 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H20" t="n">
-        <v>0.0356623108130311</v>
+        <v>0.0203099057522167</v>
       </c>
       <c r="I20" t="n">
         <v>0.0</v>
@@ -3816,13 +3816,13 @@
         <v>0.0</v>
       </c>
       <c r="K20" t="n">
-        <v>0.03171247357293869</v>
+        <v>0.07188160676532769</v>
       </c>
       <c r="L20" t="n">
         <v>0.0</v>
       </c>
       <c r="M20" t="n">
-        <v>0.0317124735729387</v>
+        <v>0.0718816067653277</v>
       </c>
       <c r="N20" t="n">
         <v>0.0</v>
@@ -3830,28 +3830,28 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="C21" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D21" t="n">
-        <v>250.0</v>
+        <v>27.0</v>
       </c>
       <c r="E21" t="n">
         <v>15.0</v>
       </c>
       <c r="F21" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G21" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="H21" t="n">
-        <v>3.12027396593513E-4</v>
+        <v>0.0356623108130311</v>
       </c>
       <c r="I21" t="n">
         <v>0.0</v>
@@ -3874,28 +3874,28 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D22" t="n">
-        <v>93.0</v>
+        <v>250.0</v>
       </c>
       <c r="E22" t="n">
-        <v>59.0</v>
+        <v>15.0</v>
       </c>
       <c r="F22" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G22" t="n">
         <v>0.0059626167965088</v>
       </c>
       <c r="H22" t="n">
-        <v>0.0204179464513697</v>
+        <v>3.12027396593513E-4</v>
       </c>
       <c r="I22" t="n">
         <v>0.0</v>
@@ -3904,13 +3904,13 @@
         <v>0.0</v>
       </c>
       <c r="K22" t="n">
-        <v>0.12473572938689217</v>
+        <v>0.03171247357293869</v>
       </c>
       <c r="L22" t="n">
         <v>0.0</v>
       </c>
       <c r="M22" t="n">
-        <v>0.124735729386892</v>
+        <v>0.0317124735729387</v>
       </c>
       <c r="N22" t="n">
         <v>0.0</v>
@@ -3918,43 +3918,43 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C23" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D23" t="n">
-        <v>158.0</v>
+        <v>103.0</v>
       </c>
       <c r="E23" t="n">
-        <v>59.0</v>
+        <v>15.0</v>
       </c>
       <c r="F23" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G23" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H23" t="n">
-        <v>0.00334798701112857</v>
+        <v>0.00167276266869532</v>
       </c>
       <c r="I23" t="n">
         <v>0.0</v>
       </c>
       <c r="J23" t="n">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
       <c r="K23" t="n">
-        <v>0.12473572938689217</v>
+        <v>0.03171247357293869</v>
       </c>
       <c r="L23" t="n">
         <v>0.0</v>
       </c>
       <c r="M23" t="n">
-        <v>0.124735729386892</v>
+        <v>0.0317124735729387</v>
       </c>
       <c r="N23" t="n">
         <v>0.0</v>
@@ -3962,43 +3962,43 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
         <v>78</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D24" t="n">
-        <v>120.0</v>
+        <v>93.0</v>
       </c>
       <c r="E24" t="n">
-        <v>82.0</v>
+        <v>59.0</v>
       </c>
       <c r="F24" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G24" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="H24" t="n">
-        <v>4.12608987825272E-4</v>
+        <v>0.0204179464513697</v>
       </c>
       <c r="I24" t="n">
         <v>0.0</v>
       </c>
       <c r="J24" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="K24" t="n">
-        <v>0.1733615221987315</v>
+        <v>0.12473572938689217</v>
       </c>
       <c r="L24" t="n">
         <v>0.0</v>
       </c>
       <c r="M24" t="n">
-        <v>0.173361522198731</v>
+        <v>0.124735729386892</v>
       </c>
       <c r="N24" t="n">
         <v>0.0</v>
@@ -4006,28 +4006,28 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D25" t="n">
-        <v>64.0</v>
+        <v>158.0</v>
       </c>
       <c r="E25" t="n">
-        <v>37.0</v>
+        <v>59.0</v>
       </c>
       <c r="F25" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G25" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H25" t="n">
-        <v>0.00333892782400472</v>
+        <v>0.00334798701112857</v>
       </c>
       <c r="I25" t="n">
         <v>0.0</v>
@@ -4036,13 +4036,13 @@
         <v>0.0</v>
       </c>
       <c r="K25" t="n">
-        <v>0.07822410147991543</v>
+        <v>0.12473572938689217</v>
       </c>
       <c r="L25" t="n">
         <v>0.0</v>
       </c>
       <c r="M25" t="n">
-        <v>0.0782241014799154</v>
+        <v>0.124735729386892</v>
       </c>
       <c r="N25" t="n">
         <v>0.0</v>
@@ -4050,16 +4050,16 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C26" t="s">
         <v>95</v>
       </c>
       <c r="D26" t="n">
-        <v>250.0</v>
+        <v>64.0</v>
       </c>
       <c r="E26" t="n">
         <v>37.0</v>
@@ -4068,10 +4068,10 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="G26" t="n">
-        <v>0.00793650793650794</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="H26" t="n">
-        <v>0.0641712118646901</v>
+        <v>0.00333892782400472</v>
       </c>
       <c r="I26" t="n">
         <v>0.0</v>
@@ -4094,28 +4094,28 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" t="s">
         <v>95</v>
       </c>
-      <c r="C27" t="s">
-        <v>96</v>
-      </c>
       <c r="D27" t="n">
+        <v>250.0</v>
+      </c>
+      <c r="E27" t="n">
         <v>37.0</v>
       </c>
-      <c r="E27" t="n">
-        <v>28.0</v>
-      </c>
       <c r="F27" t="n">
-        <v>0.0158730158730159</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G27" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.00793650793650794</v>
       </c>
       <c r="H27" t="n">
-        <v>0.015920859802431</v>
+        <v>0.0641712118646901</v>
       </c>
       <c r="I27" t="n">
         <v>0.0</v>
@@ -4124,42 +4124,42 @@
         <v>0.0</v>
       </c>
       <c r="K27" t="n">
-        <v>0.05919661733615222</v>
+        <v>0.07822410147991543</v>
       </c>
       <c r="L27" t="n">
         <v>0.0</v>
       </c>
       <c r="M27" t="n">
-        <v>0.0591966173361522</v>
+        <v>0.0782241014799154</v>
       </c>
       <c r="N27" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="C28" t="s">
         <v>96</v>
       </c>
       <c r="D28" t="n">
-        <v>46.0</v>
+        <v>37.0</v>
       </c>
       <c r="E28" t="n">
         <v>28.0</v>
       </c>
       <c r="F28" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.0158730158730159</v>
       </c>
       <c r="G28" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H28" t="n">
-        <v>0.0142728080658903</v>
+        <v>0.015920859802431</v>
       </c>
       <c r="I28" t="n">
         <v>0.0</v>
@@ -4182,28 +4182,28 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="C29" t="s">
         <v>96</v>
       </c>
       <c r="D29" t="n">
-        <v>35.0</v>
+        <v>46.0</v>
       </c>
       <c r="E29" t="n">
         <v>28.0</v>
       </c>
       <c r="F29" t="n">
-        <v>0.0468463097466241</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G29" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H29" t="n">
-        <v>0.0417860943528127</v>
+        <v>0.0142728080658903</v>
       </c>
       <c r="I29" t="n">
         <v>0.0</v>
@@ -4221,33 +4221,33 @@
         <v>0.0591966173361522</v>
       </c>
       <c r="N29" t="n">
-        <v>3.2710259555912E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B30" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" t="s">
         <v>96</v>
       </c>
-      <c r="C30" t="s">
-        <v>79</v>
-      </c>
       <c r="D30" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="E30" t="n">
         <v>28.0</v>
       </c>
-      <c r="E30" t="n">
-        <v>25.0</v>
-      </c>
       <c r="F30" t="n">
-        <v>0.0277777777777778</v>
+        <v>0.0468463097466241</v>
       </c>
       <c r="G30" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H30" t="n">
-        <v>0.00528885616238524</v>
+        <v>0.0417860943528127</v>
       </c>
       <c r="I30" t="n">
         <v>0.0</v>
@@ -4256,42 +4256,42 @@
         <v>0.0</v>
       </c>
       <c r="K30" t="n">
-        <v>0.052854122621564484</v>
+        <v>0.05919661733615222</v>
       </c>
       <c r="L30" t="n">
         <v>0.0</v>
       </c>
       <c r="M30" t="n">
-        <v>0.0528541226215645</v>
+        <v>0.0591966173361522</v>
       </c>
       <c r="N30" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B31" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D31" t="n">
-        <v>31.0</v>
+        <v>28.0</v>
       </c>
       <c r="E31" t="n">
         <v>25.0</v>
       </c>
       <c r="F31" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.0277777777777778</v>
       </c>
       <c r="G31" t="n">
-        <v>0.0158730158730159</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="H31" t="n">
-        <v>0.00130554100709877</v>
+        <v>0.00528885616238524</v>
       </c>
       <c r="I31" t="n">
         <v>0.0</v>
@@ -4303,39 +4303,39 @@
         <v>0.052854122621564484</v>
       </c>
       <c r="L31" t="n">
-        <v>0.0</v>
+        <v>3.271025955591198E-18</v>
       </c>
       <c r="M31" t="n">
         <v>0.0528541226215645</v>
       </c>
       <c r="N31" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="C32" t="s">
         <v>77</v>
       </c>
       <c r="D32" t="n">
-        <v>84.0</v>
+        <v>31.0</v>
       </c>
       <c r="E32" t="n">
-        <v>46.0</v>
+        <v>25.0</v>
       </c>
       <c r="F32" t="n">
         <v>0.0059626167965088</v>
       </c>
       <c r="G32" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0158730158730159</v>
       </c>
       <c r="H32" t="n">
-        <v>0.00153994324064719</v>
+        <v>0.00130554100709877</v>
       </c>
       <c r="I32" t="n">
         <v>0.0</v>
@@ -4344,13 +4344,13 @@
         <v>0.0</v>
       </c>
       <c r="K32" t="n">
-        <v>0.09725158562367865</v>
+        <v>0.052854122621564484</v>
       </c>
       <c r="L32" t="n">
-        <v>0.0</v>
+        <v>3.271025955591198E-18</v>
       </c>
       <c r="M32" t="n">
-        <v>0.0972515856236787</v>
+        <v>0.0528541226215645</v>
       </c>
       <c r="N32" t="n">
         <v>0.0</v>
@@ -4358,28 +4358,28 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="C33" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="D33" t="n">
-        <v>31.0</v>
+        <v>84.0</v>
       </c>
       <c r="E33" t="n">
-        <v>25.0</v>
+        <v>46.0</v>
       </c>
       <c r="F33" t="n">
-        <v>0.0172268185197356</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G33" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="H33" t="n">
-        <v>0.00352256830938948</v>
+        <v>0.00153994324064719</v>
       </c>
       <c r="I33" t="n">
         <v>0.0</v>
@@ -4388,16 +4388,16 @@
         <v>0.0</v>
       </c>
       <c r="K33" t="n">
-        <v>0.052854122621564484</v>
+        <v>0.09725158562367865</v>
       </c>
       <c r="L33" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M33" t="n">
-        <v>0.0528541226215645</v>
+        <v>0.0972515856236787</v>
       </c>
       <c r="N33" t="n">
-        <v>3.2710259555912E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="34">
@@ -4405,37 +4405,37 @@
         <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="C34" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D34" t="n">
-        <v>250.0</v>
+        <v>31.0</v>
       </c>
       <c r="E34" t="n">
         <v>25.0</v>
       </c>
       <c r="F34" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0172268185197356</v>
       </c>
       <c r="G34" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="H34" t="n">
-        <v>0.00148405904181779</v>
+        <v>0.00352256830938948</v>
       </c>
       <c r="I34" t="n">
         <v>0.0</v>
       </c>
       <c r="J34" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="K34" t="n">
         <v>0.052854122621564484</v>
       </c>
       <c r="L34" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M34" t="n">
         <v>0.0528541226215645</v>
@@ -4446,43 +4446,43 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C35" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D35" t="n">
-        <v>93.0</v>
+        <v>250.0</v>
       </c>
       <c r="E35" t="n">
-        <v>31.0</v>
+        <v>25.0</v>
       </c>
       <c r="F35" t="n">
-        <v>0.0058336561716597</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G35" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H35" t="n">
-        <v>0.0572545435376393</v>
+        <v>0.00148405904181779</v>
       </c>
       <c r="I35" t="n">
         <v>0.0</v>
       </c>
       <c r="J35" t="n">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
       <c r="K35" t="n">
-        <v>0.06553911205073996</v>
+        <v>0.052854122621564484</v>
       </c>
       <c r="L35" t="n">
-        <v>4.625929269271485E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M35" t="n">
-        <v>0.06553911205074</v>
+        <v>0.0528541226215645</v>
       </c>
       <c r="N35" t="n">
         <v>0.0</v>
@@ -4490,28 +4490,28 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C36" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="D36" t="n">
-        <v>250.0</v>
+        <v>93.0</v>
       </c>
       <c r="E36" t="n">
-        <v>64.0</v>
+        <v>31.0</v>
       </c>
       <c r="F36" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0058336561716597</v>
       </c>
       <c r="G36" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H36" t="n">
-        <v>0.0500405705476867</v>
+        <v>0.0572545435376393</v>
       </c>
       <c r="I36" t="n">
         <v>0.0</v>
@@ -4520,13 +4520,13 @@
         <v>0.0</v>
       </c>
       <c r="K36" t="n">
-        <v>0.13530655391120508</v>
+        <v>0.06553911205073996</v>
       </c>
       <c r="L36" t="n">
         <v>0.0</v>
       </c>
       <c r="M36" t="n">
-        <v>0.135306553911205</v>
+        <v>0.06553911205074</v>
       </c>
       <c r="N36" t="n">
         <v>0.0</v>
@@ -4534,28 +4534,28 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="C37" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="D37" t="n">
-        <v>37.0</v>
+        <v>250.0</v>
       </c>
       <c r="E37" t="n">
-        <v>27.0</v>
+        <v>64.0</v>
       </c>
       <c r="F37" t="n">
-        <v>0.00798534817689006</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G37" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H37" t="n">
-        <v>0.00573068158794917</v>
+        <v>0.0500405705476867</v>
       </c>
       <c r="I37" t="n">
         <v>0.0</v>
@@ -4564,13 +4564,13 @@
         <v>0.0</v>
       </c>
       <c r="K37" t="n">
-        <v>0.05708245243128964</v>
+        <v>0.13530655391120508</v>
       </c>
       <c r="L37" t="n">
         <v>0.0</v>
       </c>
       <c r="M37" t="n">
-        <v>0.0570824524312896</v>
+        <v>0.135306553911205</v>
       </c>
       <c r="N37" t="n">
         <v>0.0</v>
@@ -4578,28 +4578,28 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B38" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C38" t="s">
         <v>102</v>
       </c>
       <c r="D38" t="n">
-        <v>41.0</v>
+        <v>37.0</v>
       </c>
       <c r="E38" t="n">
         <v>27.0</v>
       </c>
       <c r="F38" t="n">
-        <v>0.00793650793650794</v>
+        <v>0.00798534817689006</v>
       </c>
       <c r="G38" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H38" t="n">
-        <v>0.00496140462033587</v>
+        <v>0.00573068158794917</v>
       </c>
       <c r="I38" t="n">
         <v>0.0</v>
@@ -4622,28 +4622,28 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B39" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C39" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="D39" t="n">
-        <v>59.0</v>
+        <v>41.0</v>
       </c>
       <c r="E39" t="n">
-        <v>31.0</v>
+        <v>27.0</v>
       </c>
       <c r="F39" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.00793650793650794</v>
       </c>
       <c r="G39" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H39" t="n">
-        <v>0.00872783618701037</v>
+        <v>0.00496140462033587</v>
       </c>
       <c r="I39" t="n">
         <v>0.0</v>
@@ -4652,30 +4652,30 @@
         <v>0.0</v>
       </c>
       <c r="K39" t="n">
-        <v>0.06553911205073996</v>
+        <v>0.05708245243128964</v>
       </c>
       <c r="L39" t="n">
-        <v>6.542051911182396E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M39" t="n">
-        <v>0.06553911205074</v>
+        <v>0.0570824524312896</v>
       </c>
       <c r="N39" t="n">
-        <v>4.62592926927149E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B40" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C40" t="s">
         <v>86</v>
       </c>
       <c r="D40" t="n">
-        <v>78.0</v>
+        <v>59.0</v>
       </c>
       <c r="E40" t="n">
         <v>31.0</v>
@@ -4687,7 +4687,7 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H40" t="n">
-        <v>0.0865916560787768</v>
+        <v>0.00872783618701037</v>
       </c>
       <c r="I40" t="n">
         <v>0.0</v>
@@ -4699,39 +4699,39 @@
         <v>0.06553911205073996</v>
       </c>
       <c r="L40" t="n">
-        <v>6.542051911182396E-18</v>
+        <v>4.625929269271485E-18</v>
       </c>
       <c r="M40" t="n">
         <v>0.06553911205074</v>
       </c>
       <c r="N40" t="n">
-        <v>0.0</v>
+        <v>6.5420519111824E-18</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B41" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C41" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="D41" t="n">
-        <v>222.0</v>
+        <v>78.0</v>
       </c>
       <c r="E41" t="n">
-        <v>37.0</v>
+        <v>31.0</v>
       </c>
       <c r="F41" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G41" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H41" t="n">
-        <v>0.00201437246540173</v>
+        <v>0.0865916560787768</v>
       </c>
       <c r="I41" t="n">
         <v>0.0</v>
@@ -4740,42 +4740,42 @@
         <v>0.0</v>
       </c>
       <c r="K41" t="n">
-        <v>0.07822410147991543</v>
+        <v>0.06553911205073996</v>
       </c>
       <c r="L41" t="n">
-        <v>0.0</v>
+        <v>4.625929269271485E-18</v>
       </c>
       <c r="M41" t="n">
-        <v>0.0782241014799154</v>
+        <v>0.06553911205074</v>
       </c>
       <c r="N41" t="n">
-        <v>0.0</v>
+        <v>6.5420519111824E-18</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>116</v>
       </c>
       <c r="C42" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="D42" t="n">
-        <v>46.0</v>
+        <v>222.0</v>
       </c>
       <c r="E42" t="n">
-        <v>23.0</v>
+        <v>37.0</v>
       </c>
       <c r="F42" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G42" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H42" t="n">
-        <v>0.145038385111565</v>
+        <v>0.00201437246540173</v>
       </c>
       <c r="I42" t="n">
         <v>0.0</v>
@@ -4784,13 +4784,13 @@
         <v>0.0</v>
       </c>
       <c r="K42" t="n">
-        <v>0.048625792811839326</v>
+        <v>0.07822410147991543</v>
       </c>
       <c r="L42" t="n">
         <v>0.0</v>
       </c>
       <c r="M42" t="n">
-        <v>0.0486257928118393</v>
+        <v>0.0782241014799154</v>
       </c>
       <c r="N42" t="n">
         <v>0.0</v>
@@ -4798,16 +4798,16 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B43" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C43" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D43" t="n">
-        <v>93.0</v>
+        <v>46.0</v>
       </c>
       <c r="E43" t="n">
         <v>23.0</v>
@@ -4816,10 +4816,10 @@
         <v>0.0059626167965088</v>
       </c>
       <c r="G43" t="n">
-        <v>0.0158730158730159</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="H43" t="n">
-        <v>0.0914870429913643</v>
+        <v>0.145038385111565</v>
       </c>
       <c r="I43" t="n">
         <v>0.0</v>
@@ -4831,7 +4831,7 @@
         <v>0.048625792811839326</v>
       </c>
       <c r="L43" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M43" t="n">
         <v>0.0486257928118393</v>
@@ -4842,40 +4842,40 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B44" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C44" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D44" t="n">
-        <v>265.0</v>
+        <v>93.0</v>
       </c>
       <c r="E44" t="n">
         <v>23.0</v>
       </c>
       <c r="F44" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G44" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0158730158730159</v>
       </c>
       <c r="H44" t="n">
-        <v>9.13202144083936E-5</v>
+        <v>0.0914870429913643</v>
       </c>
       <c r="I44" t="n">
         <v>0.0</v>
       </c>
       <c r="J44" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="K44" t="n">
         <v>0.048625792811839326</v>
       </c>
       <c r="L44" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M44" t="n">
         <v>0.0486257928118393</v>
@@ -4886,43 +4886,43 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B45" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C45" t="s">
         <v>92</v>
       </c>
       <c r="D45" t="n">
-        <v>26.0</v>
+        <v>265.0</v>
       </c>
       <c r="E45" t="n">
-        <v>26.0</v>
+        <v>23.0</v>
       </c>
       <c r="F45" t="n">
-        <v>0.0166693416357932</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G45" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H45" t="n">
-        <v>0.0165947985726984</v>
+        <v>9.13202144083936E-5</v>
       </c>
       <c r="I45" t="n">
         <v>0.0</v>
       </c>
       <c r="J45" t="n">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
       <c r="K45" t="n">
-        <v>0.05496828752642706</v>
+        <v>0.048625792811839326</v>
       </c>
       <c r="L45" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M45" t="n">
-        <v>0.0549682875264271</v>
+        <v>0.0486257928118393</v>
       </c>
       <c r="N45" t="n">
         <v>2.31296463463574E-18</v>
@@ -4930,34 +4930,34 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B46" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C46" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D46" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
       <c r="E46" t="n">
         <v>26.0</v>
       </c>
       <c r="F46" t="n">
-        <v>0.414406187123225</v>
+        <v>0.0166693416357932</v>
       </c>
       <c r="G46" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H46" t="n">
-        <v>0.00877923124276454</v>
+        <v>0.0165947985726984</v>
       </c>
       <c r="I46" t="n">
         <v>0.0</v>
       </c>
       <c r="J46" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="K46" t="n">
         <v>0.05496828752642706</v>
@@ -4966,10 +4966,10 @@
         <v>0.0</v>
       </c>
       <c r="M46" t="n">
-        <v>0.0562367864693446</v>
+        <v>0.0549682875264271</v>
       </c>
       <c r="N46" t="n">
-        <v>0.00401134586913537</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="47">
@@ -4980,7 +4980,7 @@
         <v>72</v>
       </c>
       <c r="C47" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D47" t="n">
         <v>250.0</v>
@@ -5065,10 +5065,10 @@
         <v>66</v>
       </c>
       <c r="B49" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49" t="s">
         <v>76</v>
-      </c>
-      <c r="C49" t="s">
-        <v>75</v>
       </c>
       <c r="D49" t="n">
         <v>93.0</v>
@@ -5112,7 +5112,7 @@
         <v>72</v>
       </c>
       <c r="C50" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D50" t="n">
         <v>250.0</v>
@@ -5145,7 +5145,7 @@
         <v>0.101479915433404</v>
       </c>
       <c r="N50" t="n">
-        <v>0.0</v>
+        <v>4.62592926927149E-18</v>
       </c>
     </row>
     <row r="51">
@@ -5244,7 +5244,7 @@
         <v>72</v>
       </c>
       <c r="C53" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D53" t="n">
         <v>250.0</v>
@@ -5285,7 +5285,7 @@
         <v>137</v>
       </c>
       <c r="B54" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C54" t="s">
         <v>117</v>
@@ -5332,7 +5332,7 @@
         <v>80</v>
       </c>
       <c r="C55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D55" t="e">
         <v>#NUM!</v>
@@ -5359,7 +5359,7 @@
         <v>0.0613107822410148</v>
       </c>
       <c r="L55" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M55" t="e">
         <v>#NUM!</v>
@@ -5370,7 +5370,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B56" t="s">
         <v>80</v>
@@ -5546,13 +5546,13 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B60" t="s">
         <v>80</v>
       </c>
       <c r="C60" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D60" t="e">
         <v>#NUM!</v>
@@ -5590,7 +5590,7 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B61" t="s">
         <v>80</v>
@@ -5816,7 +5816,7 @@
         <v>80</v>
       </c>
       <c r="C66" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D66" t="e">
         <v>#NUM!</v>
@@ -5884,10 +5884,10 @@
         <v>#NUM!</v>
       </c>
       <c r="K67" t="n">
-        <v>0.4885835095137421</v>
+        <v>0.48710359408033826</v>
       </c>
       <c r="L67" t="n">
-        <v>0.011382945174485744</v>
+        <v>0.009359807027982536</v>
       </c>
       <c r="M67" t="e">
         <v>#NUM!</v>
@@ -5992,7 +5992,7 @@
         <v>80</v>
       </c>
       <c r="C70" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D70" t="e">
         <v>#NUM!</v>

</xml_diff>

<commit_message>
added imports file for installing all required packages
</commit_message>
<xml_diff>
--- a/output/LUAD_statistics_all subtypes.xlsx
+++ b/output/LUAD_statistics_all subtypes.xlsx
@@ -54,60 +54,60 @@
     <t>capri_bic.SD.POSTERR</t>
   </si>
   <si>
+    <t>7</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
     <t>5</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>36</t>
+    <t>8</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
   <si>
     <t>29</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>27</t>
+    <t>35</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>31</t>
   </si>
   <si>
     <t>32</t>
   </si>
   <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -216,82 +216,82 @@
     <t>54</t>
   </si>
   <si>
+    <t>Mutation KRAS</t>
+  </si>
+  <si>
     <t>Pattern OR_CDKN2A</t>
   </si>
   <si>
+    <t>Mutation NF1</t>
+  </si>
+  <si>
+    <t>Mutation SMARCA4</t>
+  </si>
+  <si>
+    <t>Pattern OR_KRAS</t>
+  </si>
+  <si>
+    <t>Amplification CDK4</t>
+  </si>
+  <si>
     <t>Mutation EGFR</t>
   </si>
   <si>
-    <t>Mutation KRAS</t>
-  </si>
-  <si>
-    <t>Amplification CDK4</t>
-  </si>
-  <si>
-    <t>Pattern OR_KRAS</t>
+    <t>Pattern OR_CDK4_TP53</t>
+  </si>
+  <si>
+    <t>Pattern OR_EGFR_SMARCA4</t>
+  </si>
+  <si>
+    <t>Mutation ATM</t>
   </si>
   <si>
     <t>Mutation TP53</t>
   </si>
   <si>
-    <t>Mutation ATM</t>
-  </si>
-  <si>
-    <t>Pattern OR_CDK4_TP53</t>
-  </si>
-  <si>
-    <t>Pattern OR_EGFR_SMARCA4</t>
-  </si>
-  <si>
-    <t>Mutation SMARCA4</t>
+    <t>Mutation KEAP1</t>
   </si>
   <si>
     <t>Mutation ARID1B</t>
   </si>
   <si>
-    <t>Mutation KEAP1</t>
-  </si>
-  <si>
-    <t>Mutation NF1</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
+    <t>Amplification KRAS</t>
+  </si>
+  <si>
     <t>Amplification CCND1</t>
   </si>
   <si>
+    <t>Mutation NFE2L2</t>
+  </si>
+  <si>
+    <t>Mutation STK11</t>
+  </si>
+  <si>
+    <t>Amplification MDM2</t>
+  </si>
+  <si>
     <t>Amplification EGFR</t>
   </si>
   <si>
-    <t>Amplification KRAS</t>
-  </si>
-  <si>
-    <t>Amplification MDM2</t>
-  </si>
-  <si>
-    <t>Mutation STK11</t>
+    <t>Deletion CDKN2A</t>
+  </si>
+  <si>
+    <t>Amplification MET</t>
   </si>
   <si>
     <t>Mutation RB1</t>
   </si>
   <si>
-    <t>Deletion CDKN2A</t>
-  </si>
-  <si>
-    <t>Mutation NFE2L2</t>
+    <t>Mutation CDKN2A</t>
+  </si>
+  <si>
+    <t>Mutation RET</t>
   </si>
   <si>
     <t>Mutation ROS1</t>
-  </si>
-  <si>
-    <t>Amplification MET</t>
-  </si>
-  <si>
-    <t>Mutation CDKN2A</t>
-  </si>
-  <si>
-    <t>Mutation RET</t>
   </si>
   <si>
     <t>Amplification CCNE1</t>
@@ -572,10 +572,10 @@
         <v>81</v>
       </c>
       <c r="D2" t="n">
-        <v>103.0</v>
+        <v>141.0</v>
       </c>
       <c r="E2" t="n">
-        <v>19.0</v>
+        <v>34.0</v>
       </c>
       <c r="F2" t="n">
         <v>0.0059626167965088</v>
@@ -584,7 +584,7 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H2" t="n">
-        <v>8.46735787535546E-6</v>
+        <v>8.88220599278587E-4</v>
       </c>
       <c r="I2" t="n">
         <v>100.0</v>
@@ -593,13 +593,13 @@
         <v>100.0</v>
       </c>
       <c r="K2" t="n">
-        <v>0.040169133192389</v>
+        <v>0.07188160676532769</v>
       </c>
       <c r="L2" t="n">
         <v>0.0</v>
       </c>
       <c r="M2" t="n">
-        <v>0.040169133192389</v>
+        <v>0.0718816067653277</v>
       </c>
       <c r="N2" t="n">
         <v>0.0</v>
@@ -616,19 +616,19 @@
         <v>82</v>
       </c>
       <c r="D3" t="n">
-        <v>65.0</v>
+        <v>103.0</v>
       </c>
       <c r="E3" t="n">
-        <v>28.0</v>
+        <v>19.0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0058336561716597</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G3" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H3" t="n">
-        <v>3.24651120035433E-13</v>
+        <v>8.46735787535546E-6</v>
       </c>
       <c r="I3" t="n">
         <v>80.0</v>
@@ -637,16 +637,16 @@
         <v>100.0</v>
       </c>
       <c r="K3" t="n">
-        <v>0.05919661733615222</v>
+        <v>0.04059196617336152</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0</v>
+        <v>0.0013371152897117902</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0591966173361522</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="N3" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
@@ -657,22 +657,22 @@
         <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D4" t="n">
-        <v>141.0</v>
+        <v>64.0</v>
       </c>
       <c r="E4" t="n">
-        <v>34.0</v>
+        <v>25.0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G4" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0158730158730159</v>
       </c>
       <c r="H4" t="n">
-        <v>8.88220599278587E-4</v>
+        <v>0.0103051123549064</v>
       </c>
       <c r="I4" t="n">
         <v>80.0</v>
@@ -681,16 +681,16 @@
         <v>100.0</v>
       </c>
       <c r="K4" t="n">
-        <v>0.07188160676532769</v>
+        <v>0.052854122621564484</v>
       </c>
       <c r="L4" t="n">
         <v>0.0</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0718816067653277</v>
+        <v>0.0528541226215645</v>
       </c>
       <c r="N4" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="5">
@@ -701,22 +701,22 @@
         <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D5" t="n">
-        <v>29.0</v>
+        <v>48.0</v>
       </c>
       <c r="E5" t="n">
-        <v>26.0</v>
+        <v>15.0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0177894166197971</v>
+        <v>0.0058336561716597</v>
       </c>
       <c r="G5" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H5" t="n">
-        <v>3.80945122355267E-7</v>
+        <v>0.00161509241969472</v>
       </c>
       <c r="I5" t="n">
         <v>80.0</v>
@@ -725,16 +725,16 @@
         <v>100.0</v>
       </c>
       <c r="K5" t="n">
-        <v>0.05496828752642706</v>
+        <v>0.03171247357293869</v>
       </c>
       <c r="L5" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0549682875264271</v>
+        <v>0.0317124735729387</v>
       </c>
       <c r="N5" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
@@ -745,7 +745,7 @@
         <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D6" t="n">
         <v>158.0</v>
@@ -769,10 +769,10 @@
         <v>100.0</v>
       </c>
       <c r="K6" t="n">
-        <v>0.17758985200845667</v>
+        <v>0.179492600422833</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0</v>
+        <v>0.004722160836575322</v>
       </c>
       <c r="M6" t="n">
         <v>0.177589852008457</v>
@@ -789,22 +789,22 @@
         <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7" t="n">
-        <v>250.0</v>
+        <v>29.0</v>
       </c>
       <c r="E7" t="n">
-        <v>31.0</v>
+        <v>26.0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.0177894166197971</v>
       </c>
       <c r="G7" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H7" t="n">
-        <v>1.07101678627571E-5</v>
+        <v>3.80945122355267E-7</v>
       </c>
       <c r="I7" t="n">
         <v>60.0</v>
@@ -813,16 +813,16 @@
         <v>100.0</v>
       </c>
       <c r="K7" t="n">
-        <v>0.06553911205073996</v>
+        <v>0.05496828752642706</v>
       </c>
       <c r="L7" t="n">
-        <v>4.625929269271485E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M7" t="n">
-        <v>0.06553911205074</v>
+        <v>0.0549682875264271</v>
       </c>
       <c r="N7" t="n">
-        <v>4.62592926927149E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="8">
@@ -833,13 +833,13 @@
         <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D8" t="n">
-        <v>46.0</v>
+        <v>65.0</v>
       </c>
       <c r="E8" t="n">
-        <v>19.0</v>
+        <v>28.0</v>
       </c>
       <c r="F8" t="n">
         <v>0.0058336561716597</v>
@@ -848,7 +848,7 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H8" t="n">
-        <v>0.00699258708471991</v>
+        <v>3.24651120035433E-13</v>
       </c>
       <c r="I8" t="n">
         <v>40.0</v>
@@ -857,13 +857,13 @@
         <v>100.0</v>
       </c>
       <c r="K8" t="n">
-        <v>0.040169133192389</v>
+        <v>0.05919661733615222</v>
       </c>
       <c r="L8" t="n">
         <v>0.0</v>
       </c>
       <c r="M8" t="n">
-        <v>0.040169133192389</v>
+        <v>0.0591966173361522</v>
       </c>
       <c r="N8" t="n">
         <v>0.0</v>
@@ -877,13 +877,13 @@
         <v>74</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D9" t="n">
         <v>265.0</v>
       </c>
       <c r="E9" t="n">
-        <v>28.0</v>
+        <v>34.0</v>
       </c>
       <c r="F9" t="n">
         <v>0.0059626167965088</v>
@@ -892,7 +892,7 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H9" t="n">
-        <v>1.77721953788421E-6</v>
+        <v>8.27584277446678E-5</v>
       </c>
       <c r="I9" t="n">
         <v>40.0</v>
@@ -901,13 +901,13 @@
         <v>100.0</v>
       </c>
       <c r="K9" t="n">
-        <v>0.05919661733615222</v>
+        <v>0.07188160676532769</v>
       </c>
       <c r="L9" t="n">
         <v>0.0</v>
       </c>
       <c r="M9" t="n">
-        <v>0.0591966173361522</v>
+        <v>0.0718816067653277</v>
       </c>
       <c r="N9" t="n">
         <v>0.0</v>
@@ -918,25 +918,25 @@
         <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D10" t="n">
-        <v>265.0</v>
+        <v>120.0</v>
       </c>
       <c r="E10" t="n">
-        <v>34.0</v>
+        <v>82.0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G10" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H10" t="n">
-        <v>8.27584277446678E-5</v>
+        <v>4.12608987825272E-4</v>
       </c>
       <c r="I10" t="n">
         <v>40.0</v>
@@ -945,13 +945,13 @@
         <v>100.0</v>
       </c>
       <c r="K10" t="n">
-        <v>0.07188160676532769</v>
+        <v>0.1733615221987315</v>
       </c>
       <c r="L10" t="n">
         <v>0.0</v>
       </c>
       <c r="M10" t="n">
-        <v>0.0718816067653277</v>
+        <v>0.173361522198731</v>
       </c>
       <c r="N10" t="n">
         <v>0.0</v>
@@ -962,25 +962,25 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D11" t="n">
-        <v>120.0</v>
+        <v>158.0</v>
       </c>
       <c r="E11" t="n">
-        <v>82.0</v>
+        <v>46.0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0058336561716597</v>
       </c>
       <c r="G11" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H11" t="n">
-        <v>4.12608987825272E-4</v>
+        <v>0.00131454955057744</v>
       </c>
       <c r="I11" t="n">
         <v>40.0</v>
@@ -989,13 +989,13 @@
         <v>100.0</v>
       </c>
       <c r="K11" t="n">
-        <v>0.1733615221987315</v>
+        <v>0.09725158562367865</v>
       </c>
       <c r="L11" t="n">
         <v>0.0</v>
       </c>
       <c r="M11" t="n">
-        <v>0.173361522198731</v>
+        <v>0.0972515856236787</v>
       </c>
       <c r="N11" t="n">
         <v>0.0</v>
@@ -1009,13 +1009,13 @@
         <v>76</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D12" t="n">
-        <v>48.0</v>
+        <v>46.0</v>
       </c>
       <c r="E12" t="n">
-        <v>15.0</v>
+        <v>19.0</v>
       </c>
       <c r="F12" t="n">
         <v>0.0058336561716597</v>
@@ -1024,22 +1024,22 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H12" t="n">
-        <v>0.00161509241969472</v>
+        <v>0.00699258708471991</v>
       </c>
       <c r="I12" t="n">
-        <v>40.0</v>
+        <v>20.0</v>
       </c>
       <c r="J12" t="n">
         <v>100.0</v>
       </c>
       <c r="K12" t="n">
-        <v>0.03171247357293869</v>
+        <v>0.04059196617336152</v>
       </c>
       <c r="L12" t="n">
-        <v>0.0</v>
+        <v>0.0013371152897117902</v>
       </c>
       <c r="M12" t="n">
-        <v>0.0317124735729387</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="N12" t="n">
         <v>0.0</v>
@@ -1050,43 +1050,43 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D13" t="n">
-        <v>25.0</v>
+        <v>265.0</v>
       </c>
       <c r="E13" t="n">
-        <v>26.0</v>
+        <v>28.0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.414406187123225</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G13" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H13" t="n">
-        <v>0.00877923124276454</v>
+        <v>1.77721953788421E-6</v>
       </c>
       <c r="I13" t="n">
-        <v>40.0</v>
+        <v>20.0</v>
       </c>
       <c r="J13" t="n">
         <v>100.0</v>
       </c>
       <c r="K13" t="n">
-        <v>0.05496828752642706</v>
+        <v>0.05919661733615222</v>
       </c>
       <c r="L13" t="n">
         <v>0.0</v>
       </c>
       <c r="M13" t="n">
-        <v>0.0549682875264271</v>
+        <v>0.0591966173361522</v>
       </c>
       <c r="N13" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="14">
@@ -1094,40 +1094,40 @@
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D14" t="n">
-        <v>93.0</v>
+        <v>103.0</v>
       </c>
       <c r="E14" t="n">
-        <v>84.0</v>
+        <v>15.0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.200982679178368</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G14" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H14" t="n">
-        <v>3.59155834889592E-4</v>
+        <v>0.00167276266869532</v>
       </c>
       <c r="I14" t="n">
-        <v>40.0</v>
+        <v>20.0</v>
       </c>
       <c r="J14" t="n">
         <v>100.0</v>
       </c>
       <c r="K14" t="n">
-        <v>0.17758985200845667</v>
+        <v>0.03171247357293869</v>
       </c>
       <c r="L14" t="n">
         <v>0.0</v>
       </c>
       <c r="M14" t="n">
-        <v>0.177589852008457</v>
+        <v>0.0317124735729387</v>
       </c>
       <c r="N14" t="n">
         <v>0.0</v>
@@ -1138,25 +1138,25 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="D15" t="n">
-        <v>64.0</v>
+        <v>250.0</v>
       </c>
       <c r="E15" t="n">
-        <v>25.0</v>
+        <v>31.0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0158730158730159</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="H15" t="n">
-        <v>0.0103051123549064</v>
+        <v>1.07101678627571E-5</v>
       </c>
       <c r="I15" t="n">
         <v>20.0</v>
@@ -1165,13 +1165,13 @@
         <v>100.0</v>
       </c>
       <c r="K15" t="n">
-        <v>0.052854122621564484</v>
+        <v>0.06553911205073996</v>
       </c>
       <c r="L15" t="n">
-        <v>3.271025955591198E-18</v>
+        <v>4.625929269271485E-18</v>
       </c>
       <c r="M15" t="n">
-        <v>0.0528541226215645</v>
+        <v>0.06553911205074</v>
       </c>
       <c r="N15" t="n">
         <v>0.0</v>
@@ -1182,25 +1182,25 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="D16" t="n">
-        <v>158.0</v>
+        <v>93.0</v>
       </c>
       <c r="E16" t="n">
-        <v>46.0</v>
+        <v>84.0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0058336561716597</v>
+        <v>0.200982679178368</v>
       </c>
       <c r="G16" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H16" t="n">
-        <v>0.00131454955057744</v>
+        <v>3.59155834889592E-4</v>
       </c>
       <c r="I16" t="n">
         <v>20.0</v>
@@ -1209,13 +1209,13 @@
         <v>100.0</v>
       </c>
       <c r="K16" t="n">
-        <v>0.09725158562367865</v>
+        <v>0.179492600422833</v>
       </c>
       <c r="L16" t="n">
-        <v>0.0</v>
+        <v>0.004722160836575322</v>
       </c>
       <c r="M16" t="n">
-        <v>0.0972515856236787</v>
+        <v>0.177589852008457</v>
       </c>
       <c r="N16" t="n">
         <v>0.0</v>
@@ -1226,16 +1226,16 @@
         <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
         <v>90</v>
       </c>
       <c r="D17" t="n">
-        <v>103.0</v>
+        <v>250.0</v>
       </c>
       <c r="E17" t="n">
-        <v>15.0</v>
+        <v>25.0</v>
       </c>
       <c r="F17" t="n">
         <v>0.00396825396825397</v>
@@ -1244,7 +1244,7 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H17" t="n">
-        <v>0.00167276266869532</v>
+        <v>0.00148405904181779</v>
       </c>
       <c r="I17" t="n">
         <v>0.0</v>
@@ -1253,13 +1253,13 @@
         <v>100.0</v>
       </c>
       <c r="K17" t="n">
-        <v>0.03171247357293869</v>
+        <v>0.052854122621564484</v>
       </c>
       <c r="L17" t="n">
         <v>0.0</v>
       </c>
       <c r="M17" t="n">
-        <v>0.0317124735729387</v>
+        <v>0.0528541226215645</v>
       </c>
       <c r="N17" t="n">
         <v>0.0</v>
@@ -1270,16 +1270,16 @@
         <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C18" t="s">
         <v>91</v>
       </c>
       <c r="D18" t="n">
-        <v>250.0</v>
+        <v>265.0</v>
       </c>
       <c r="E18" t="n">
-        <v>25.0</v>
+        <v>23.0</v>
       </c>
       <c r="F18" t="n">
         <v>0.00396825396825397</v>
@@ -1288,7 +1288,7 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H18" t="n">
-        <v>0.00148405904181779</v>
+        <v>9.13202144083936E-5</v>
       </c>
       <c r="I18" t="n">
         <v>0.0</v>
@@ -1297,16 +1297,16 @@
         <v>100.0</v>
       </c>
       <c r="K18" t="n">
-        <v>0.052854122621564484</v>
+        <v>0.048625792811839326</v>
       </c>
       <c r="L18" t="n">
         <v>0.0</v>
       </c>
       <c r="M18" t="n">
-        <v>0.0528541226215645</v>
+        <v>0.0486257928118393</v>
       </c>
       <c r="N18" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="19">
@@ -1314,25 +1314,25 @@
         <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
         <v>92</v>
       </c>
       <c r="D19" t="n">
-        <v>265.0</v>
+        <v>25.0</v>
       </c>
       <c r="E19" t="n">
-        <v>23.0</v>
+        <v>26.0</v>
       </c>
       <c r="F19" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.414406187123225</v>
       </c>
       <c r="G19" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H19" t="n">
-        <v>9.13202144083936E-5</v>
+        <v>0.00877923124276454</v>
       </c>
       <c r="I19" t="n">
         <v>0.0</v>
@@ -1341,13 +1341,13 @@
         <v>100.0</v>
       </c>
       <c r="K19" t="n">
-        <v>0.048625792811839326</v>
+        <v>0.05496828752642706</v>
       </c>
       <c r="L19" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M19" t="n">
-        <v>0.0486257928118393</v>
+        <v>0.0549682875264271</v>
       </c>
       <c r="N19" t="n">
         <v>2.31296463463574E-18</v>
@@ -1388,7 +1388,7 @@
         <v>0.05708245243128964</v>
       </c>
       <c r="L20" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M20" t="e">
         <v>#NUM!</v>
@@ -1405,7 +1405,7 @@
         <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D21" t="e">
         <v>#NUM!</v>
@@ -1432,7 +1432,7 @@
         <v>0.0613107822410148</v>
       </c>
       <c r="L21" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M21" t="e">
         <v>#NUM!</v>
@@ -1669,7 +1669,7 @@
         <v>80</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D27" t="e">
         <v>#NUM!</v>
@@ -1801,7 +1801,7 @@
         <v>80</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D30" t="e">
         <v>#NUM!</v>
@@ -1916,7 +1916,7 @@
         <v>0.06553911205073996</v>
       </c>
       <c r="L32" t="n">
-        <v>0.0</v>
+        <v>4.625929269271485E-18</v>
       </c>
       <c r="M32" t="e">
         <v>#NUM!</v>
@@ -1933,7 +1933,7 @@
         <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D33" t="e">
         <v>#NUM!</v>
@@ -2109,7 +2109,7 @@
         <v>80</v>
       </c>
       <c r="C37" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D37" t="e">
         <v>#NUM!</v>
@@ -2153,7 +2153,7 @@
         <v>80</v>
       </c>
       <c r="C38" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D38" t="e">
         <v>#NUM!</v>
@@ -2329,7 +2329,7 @@
         <v>80</v>
       </c>
       <c r="C42" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D42" t="e">
         <v>#NUM!</v>
@@ -2441,10 +2441,10 @@
         <v>#NUM!</v>
       </c>
       <c r="K44" t="n">
-        <v>0.48710359408033826</v>
+        <v>0.49577167019027485</v>
       </c>
       <c r="L44" t="n">
-        <v>0.009359807027982536</v>
+        <v>0.018863648786926254</v>
       </c>
       <c r="M44" t="e">
         <v>#NUM!</v>
@@ -2994,7 +2994,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>67</v>
@@ -3003,10 +3003,10 @@
         <v>81</v>
       </c>
       <c r="D2" t="n">
-        <v>103.0</v>
+        <v>141.0</v>
       </c>
       <c r="E2" t="n">
-        <v>19.0</v>
+        <v>34.0</v>
       </c>
       <c r="F2" t="n">
         <v>0.0059626167965088</v>
@@ -3015,7 +3015,7 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H2" t="n">
-        <v>8.46735787535546E-6</v>
+        <v>8.88220599278587E-4</v>
       </c>
       <c r="I2" t="n">
         <v>100.0</v>
@@ -3024,13 +3024,13 @@
         <v>100.0</v>
       </c>
       <c r="K2" t="n">
-        <v>0.040169133192389</v>
+        <v>0.07188160676532769</v>
       </c>
       <c r="L2" t="n">
         <v>0.0</v>
       </c>
       <c r="M2" t="n">
-        <v>0.040169133192389</v>
+        <v>0.0718816067653277</v>
       </c>
       <c r="N2" t="n">
         <v>0.0</v>
@@ -3038,7 +3038,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>68</v>
@@ -3047,19 +3047,19 @@
         <v>82</v>
       </c>
       <c r="D3" t="n">
-        <v>65.0</v>
+        <v>103.0</v>
       </c>
       <c r="E3" t="n">
-        <v>28.0</v>
+        <v>19.0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0058336561716597</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G3" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H3" t="n">
-        <v>3.24651120035433E-13</v>
+        <v>8.46735787535546E-6</v>
       </c>
       <c r="I3" t="n">
         <v>80.0</v>
@@ -3068,42 +3068,42 @@
         <v>100.0</v>
       </c>
       <c r="K3" t="n">
-        <v>0.05919661733615222</v>
+        <v>0.04059196617336152</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0</v>
+        <v>0.0013371152897117902</v>
       </c>
       <c r="M3" t="n">
-        <v>0.126427061310782</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="N3" t="n">
-        <v>0.00579416625541775</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
         <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D4" t="n">
-        <v>141.0</v>
+        <v>64.0</v>
       </c>
       <c r="E4" t="n">
-        <v>34.0</v>
+        <v>25.0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G4" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0158730158730159</v>
       </c>
       <c r="H4" t="n">
-        <v>8.88220599278587E-4</v>
+        <v>0.0103051123549064</v>
       </c>
       <c r="I4" t="n">
         <v>80.0</v>
@@ -3112,13 +3112,13 @@
         <v>100.0</v>
       </c>
       <c r="K4" t="n">
-        <v>0.07188160676532769</v>
+        <v>0.052854122621564484</v>
       </c>
       <c r="L4" t="n">
         <v>0.0</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0718816067653277</v>
+        <v>0.0528541226215645</v>
       </c>
       <c r="N4" t="n">
         <v>0.0</v>
@@ -3126,28 +3126,28 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
         <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D5" t="n">
-        <v>29.0</v>
+        <v>48.0</v>
       </c>
       <c r="E5" t="n">
-        <v>26.0</v>
+        <v>15.0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0177894166197971</v>
+        <v>0.0058336561716597</v>
       </c>
       <c r="G5" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H5" t="n">
-        <v>3.80945122355267E-7</v>
+        <v>0.00161509241969472</v>
       </c>
       <c r="I5" t="n">
         <v>80.0</v>
@@ -3156,16 +3156,16 @@
         <v>100.0</v>
       </c>
       <c r="K5" t="n">
-        <v>0.05496828752642706</v>
+        <v>0.03171247357293869</v>
       </c>
       <c r="L5" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0558139534883721</v>
+        <v>0.0317124735729387</v>
       </c>
       <c r="N5" t="n">
-        <v>0.00267423057942358</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
@@ -3176,7 +3176,7 @@
         <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D6" t="n">
         <v>158.0</v>
@@ -3200,10 +3200,10 @@
         <v>100.0</v>
       </c>
       <c r="K6" t="n">
-        <v>0.17758985200845667</v>
+        <v>0.179492600422833</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0</v>
+        <v>0.004722160836575322</v>
       </c>
       <c r="M6" t="n">
         <v>0.177589852008457</v>
@@ -3214,28 +3214,28 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7" t="n">
-        <v>250.0</v>
+        <v>29.0</v>
       </c>
       <c r="E7" t="n">
-        <v>31.0</v>
+        <v>26.0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.0177894166197971</v>
       </c>
       <c r="G7" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H7" t="n">
-        <v>1.07101678627571E-5</v>
+        <v>3.80945122355267E-7</v>
       </c>
       <c r="I7" t="n">
         <v>60.0</v>
@@ -3244,13 +3244,13 @@
         <v>100.0</v>
       </c>
       <c r="K7" t="n">
-        <v>0.06553911205073996</v>
+        <v>0.05496828752642706</v>
       </c>
       <c r="L7" t="n">
-        <v>4.625929269271485E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M7" t="n">
-        <v>0.06553911205074</v>
+        <v>0.0549682875264271</v>
       </c>
       <c r="N7" t="n">
         <v>0.0</v>
@@ -3258,19 +3258,19 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
         <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D8" t="n">
-        <v>46.0</v>
+        <v>65.0</v>
       </c>
       <c r="E8" t="n">
-        <v>19.0</v>
+        <v>28.0</v>
       </c>
       <c r="F8" t="n">
         <v>0.0058336561716597</v>
@@ -3279,7 +3279,7 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H8" t="n">
-        <v>0.00699258708471991</v>
+        <v>3.24651120035433E-13</v>
       </c>
       <c r="I8" t="n">
         <v>40.0</v>
@@ -3288,33 +3288,33 @@
         <v>100.0</v>
       </c>
       <c r="K8" t="n">
-        <v>0.040169133192389</v>
+        <v>0.05919661733615222</v>
       </c>
       <c r="L8" t="n">
         <v>0.0</v>
       </c>
       <c r="M8" t="n">
-        <v>0.040169133192389</v>
+        <v>0.124947145877378</v>
       </c>
       <c r="N8" t="n">
-        <v>0.0</v>
+        <v>0.00416322917202027</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
         <v>74</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D9" t="n">
         <v>265.0</v>
       </c>
       <c r="E9" t="n">
-        <v>28.0</v>
+        <v>34.0</v>
       </c>
       <c r="F9" t="n">
         <v>0.0059626167965088</v>
@@ -3323,7 +3323,7 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H9" t="n">
-        <v>1.77721953788421E-6</v>
+        <v>8.27584277446678E-5</v>
       </c>
       <c r="I9" t="n">
         <v>40.0</v>
@@ -3332,42 +3332,42 @@
         <v>100.0</v>
       </c>
       <c r="K9" t="n">
-        <v>0.05919661733615222</v>
+        <v>0.07188160676532769</v>
       </c>
       <c r="L9" t="n">
         <v>0.0</v>
       </c>
       <c r="M9" t="n">
-        <v>0.0591966173361522</v>
+        <v>0.0718816067653277</v>
       </c>
       <c r="N9" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D10" t="n">
-        <v>265.0</v>
+        <v>120.0</v>
       </c>
       <c r="E10" t="n">
-        <v>34.0</v>
+        <v>82.0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G10" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H10" t="n">
-        <v>8.27584277446678E-5</v>
+        <v>4.12608987825272E-4</v>
       </c>
       <c r="I10" t="n">
         <v>40.0</v>
@@ -3376,13 +3376,13 @@
         <v>100.0</v>
       </c>
       <c r="K10" t="n">
-        <v>0.07188160676532769</v>
+        <v>0.1733615221987315</v>
       </c>
       <c r="L10" t="n">
         <v>0.0</v>
       </c>
       <c r="M10" t="n">
-        <v>0.0718816067653277</v>
+        <v>0.173361522198731</v>
       </c>
       <c r="N10" t="n">
         <v>0.0</v>
@@ -3390,28 +3390,28 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D11" t="n">
-        <v>120.0</v>
+        <v>158.0</v>
       </c>
       <c r="E11" t="n">
-        <v>82.0</v>
+        <v>46.0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0058336561716597</v>
       </c>
       <c r="G11" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H11" t="n">
-        <v>4.12608987825272E-4</v>
+        <v>0.00131454955057744</v>
       </c>
       <c r="I11" t="n">
         <v>40.0</v>
@@ -3420,13 +3420,13 @@
         <v>100.0</v>
       </c>
       <c r="K11" t="n">
-        <v>0.1733615221987315</v>
+        <v>0.09725158562367865</v>
       </c>
       <c r="L11" t="n">
         <v>0.0</v>
       </c>
       <c r="M11" t="n">
-        <v>0.173361522198731</v>
+        <v>0.0972515856236787</v>
       </c>
       <c r="N11" t="n">
         <v>0.0</v>
@@ -3434,19 +3434,19 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
         <v>76</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D12" t="n">
-        <v>48.0</v>
+        <v>46.0</v>
       </c>
       <c r="E12" t="n">
-        <v>15.0</v>
+        <v>19.0</v>
       </c>
       <c r="F12" t="n">
         <v>0.0058336561716597</v>
@@ -3455,22 +3455,22 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H12" t="n">
-        <v>0.00161509241969472</v>
+        <v>0.00699258708471991</v>
       </c>
       <c r="I12" t="n">
-        <v>40.0</v>
+        <v>20.0</v>
       </c>
       <c r="J12" t="n">
         <v>100.0</v>
       </c>
       <c r="K12" t="n">
-        <v>0.03171247357293869</v>
+        <v>0.04059196617336152</v>
       </c>
       <c r="L12" t="n">
-        <v>0.0</v>
+        <v>0.0013371152897117902</v>
       </c>
       <c r="M12" t="n">
-        <v>0.0317124735729387</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="N12" t="n">
         <v>0.0</v>
@@ -3478,87 +3478,87 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D13" t="n">
-        <v>25.0</v>
+        <v>265.0</v>
       </c>
       <c r="E13" t="n">
-        <v>26.0</v>
+        <v>28.0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.414406187123225</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G13" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H13" t="n">
-        <v>0.00877923124276454</v>
+        <v>1.77721953788421E-6</v>
       </c>
       <c r="I13" t="n">
-        <v>40.0</v>
+        <v>20.0</v>
       </c>
       <c r="J13" t="n">
         <v>100.0</v>
       </c>
       <c r="K13" t="n">
-        <v>0.05496828752642706</v>
+        <v>0.05919661733615222</v>
       </c>
       <c r="L13" t="n">
         <v>0.0</v>
       </c>
       <c r="M13" t="n">
-        <v>0.0551797040169133</v>
+        <v>0.0591966173361522</v>
       </c>
       <c r="N13" t="n">
-        <v>6.68557644855895E-4</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>132</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D14" t="n">
-        <v>93.0</v>
+        <v>103.0</v>
       </c>
       <c r="E14" t="n">
-        <v>84.0</v>
+        <v>15.0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.200982679178368</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G14" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H14" t="n">
-        <v>3.59155834889592E-4</v>
+        <v>0.00167276266869532</v>
       </c>
       <c r="I14" t="n">
-        <v>40.0</v>
+        <v>20.0</v>
       </c>
       <c r="J14" t="n">
         <v>100.0</v>
       </c>
       <c r="K14" t="n">
-        <v>0.17758985200845667</v>
+        <v>0.03171247357293869</v>
       </c>
       <c r="L14" t="n">
         <v>0.0</v>
       </c>
       <c r="M14" t="n">
-        <v>0.177589852008457</v>
+        <v>0.0317124735729387</v>
       </c>
       <c r="N14" t="n">
         <v>0.0</v>
@@ -3566,28 +3566,28 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="D15" t="n">
-        <v>64.0</v>
+        <v>250.0</v>
       </c>
       <c r="E15" t="n">
-        <v>25.0</v>
+        <v>31.0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0158730158730159</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="H15" t="n">
-        <v>0.0103051123549064</v>
+        <v>1.07101678627571E-5</v>
       </c>
       <c r="I15" t="n">
         <v>20.0</v>
@@ -3596,42 +3596,42 @@
         <v>100.0</v>
       </c>
       <c r="K15" t="n">
-        <v>0.052854122621564484</v>
+        <v>0.06553911205073996</v>
       </c>
       <c r="L15" t="n">
-        <v>3.271025955591198E-18</v>
+        <v>4.625929269271485E-18</v>
       </c>
       <c r="M15" t="n">
-        <v>0.0528541226215645</v>
+        <v>0.06553911205074</v>
       </c>
       <c r="N15" t="n">
-        <v>0.0</v>
+        <v>6.5420519111824E-18</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>132</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="D16" t="n">
-        <v>158.0</v>
+        <v>93.0</v>
       </c>
       <c r="E16" t="n">
-        <v>46.0</v>
+        <v>84.0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0058336561716597</v>
+        <v>0.200982679178368</v>
       </c>
       <c r="G16" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H16" t="n">
-        <v>0.00131454955057744</v>
+        <v>3.59155834889592E-4</v>
       </c>
       <c r="I16" t="n">
         <v>20.0</v>
@@ -3640,13 +3640,13 @@
         <v>100.0</v>
       </c>
       <c r="K16" t="n">
-        <v>0.09725158562367865</v>
+        <v>0.179492600422833</v>
       </c>
       <c r="L16" t="n">
-        <v>0.0</v>
+        <v>0.004722160836575322</v>
       </c>
       <c r="M16" t="n">
-        <v>0.0972515856236787</v>
+        <v>0.177589852008457</v>
       </c>
       <c r="N16" t="n">
         <v>0.0</v>
@@ -3654,13 +3654,13 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D17" t="n">
         <v>48.0</v>
@@ -3684,10 +3684,10 @@
         <v>0.0</v>
       </c>
       <c r="K17" t="n">
-        <v>0.040169133192389</v>
+        <v>0.04059196617336152</v>
       </c>
       <c r="L17" t="n">
-        <v>0.0</v>
+        <v>0.0013371152897117902</v>
       </c>
       <c r="M17" t="n">
         <v>0.040169133192389</v>
@@ -3701,7 +3701,7 @@
         <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
         <v>93</v>
@@ -3731,7 +3731,7 @@
         <v>0.05708245243128964</v>
       </c>
       <c r="L18" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M18" t="n">
         <v>0.0570824524312896</v>
@@ -3742,13 +3742,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
         <v>113</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D19" t="n">
         <v>266.0</v>
@@ -3778,21 +3778,21 @@
         <v>0.0</v>
       </c>
       <c r="M19" t="n">
-        <v>0.0591966173361522</v>
+        <v>0.0638477801268499</v>
       </c>
       <c r="N19" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0147082681868297</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D20" t="n">
         <v>250.0</v>
@@ -3836,7 +3836,7 @@
         <v>93</v>
       </c>
       <c r="C21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D21" t="n">
         <v>27.0</v>
@@ -3877,10 +3877,10 @@
         <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D22" t="n">
         <v>250.0</v>
@@ -3918,43 +3918,43 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C23" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D23" t="n">
-        <v>103.0</v>
+        <v>93.0</v>
       </c>
       <c r="E23" t="n">
-        <v>15.0</v>
+        <v>59.0</v>
       </c>
       <c r="F23" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G23" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="H23" t="n">
-        <v>0.00167276266869532</v>
+        <v>0.0204179464513697</v>
       </c>
       <c r="I23" t="n">
         <v>0.0</v>
       </c>
       <c r="J23" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="K23" t="n">
-        <v>0.03171247357293869</v>
+        <v>0.12473572938689217</v>
       </c>
       <c r="L23" t="n">
         <v>0.0</v>
       </c>
       <c r="M23" t="n">
-        <v>0.0317124735729387</v>
+        <v>0.124735729386892</v>
       </c>
       <c r="N23" t="n">
         <v>0.0</v>
@@ -3962,16 +3962,16 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C24" t="s">
         <v>94</v>
       </c>
       <c r="D24" t="n">
-        <v>93.0</v>
+        <v>158.0</v>
       </c>
       <c r="E24" t="n">
         <v>59.0</v>
@@ -3980,10 +3980,10 @@
         <v>0.0059626167965088</v>
       </c>
       <c r="G24" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="H24" t="n">
-        <v>0.0204179464513697</v>
+        <v>0.00334798701112857</v>
       </c>
       <c r="I24" t="n">
         <v>0.0</v>
@@ -4001,33 +4001,33 @@
         <v>0.124735729386892</v>
       </c>
       <c r="N24" t="n">
-        <v>0.0</v>
+        <v>4.62592926927149E-18</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C25" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D25" t="n">
-        <v>158.0</v>
+        <v>64.0</v>
       </c>
       <c r="E25" t="n">
-        <v>59.0</v>
+        <v>37.0</v>
       </c>
       <c r="F25" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G25" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H25" t="n">
-        <v>0.00334798701112857</v>
+        <v>0.00333892782400472</v>
       </c>
       <c r="I25" t="n">
         <v>0.0</v>
@@ -4036,13 +4036,13 @@
         <v>0.0</v>
       </c>
       <c r="K25" t="n">
-        <v>0.12473572938689217</v>
+        <v>0.07822410147991543</v>
       </c>
       <c r="L25" t="n">
         <v>0.0</v>
       </c>
       <c r="M25" t="n">
-        <v>0.124735729386892</v>
+        <v>0.0782241014799154</v>
       </c>
       <c r="N25" t="n">
         <v>0.0</v>
@@ -4050,16 +4050,16 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C26" t="s">
         <v>95</v>
       </c>
       <c r="D26" t="n">
-        <v>64.0</v>
+        <v>250.0</v>
       </c>
       <c r="E26" t="n">
         <v>37.0</v>
@@ -4068,10 +4068,10 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="G26" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.00793650793650794</v>
       </c>
       <c r="H26" t="n">
-        <v>0.00333892782400472</v>
+        <v>0.0641712118646901</v>
       </c>
       <c r="I26" t="n">
         <v>0.0</v>
@@ -4094,28 +4094,28 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="C27" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D27" t="n">
-        <v>250.0</v>
+        <v>37.0</v>
       </c>
       <c r="E27" t="n">
-        <v>37.0</v>
+        <v>28.0</v>
       </c>
       <c r="F27" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0158730158730159</v>
       </c>
       <c r="G27" t="n">
-        <v>0.00793650793650794</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="H27" t="n">
-        <v>0.0641712118646901</v>
+        <v>0.015920859802431</v>
       </c>
       <c r="I27" t="n">
         <v>0.0</v>
@@ -4124,42 +4124,42 @@
         <v>0.0</v>
       </c>
       <c r="K27" t="n">
-        <v>0.07822410147991543</v>
+        <v>0.05919661733615222</v>
       </c>
       <c r="L27" t="n">
         <v>0.0</v>
       </c>
       <c r="M27" t="n">
-        <v>0.0782241014799154</v>
+        <v>0.0591966173361522</v>
       </c>
       <c r="N27" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="C28" t="s">
         <v>96</v>
       </c>
       <c r="D28" t="n">
-        <v>37.0</v>
+        <v>46.0</v>
       </c>
       <c r="E28" t="n">
         <v>28.0</v>
       </c>
       <c r="F28" t="n">
-        <v>0.0158730158730159</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G28" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H28" t="n">
-        <v>0.015920859802431</v>
+        <v>0.0142728080658903</v>
       </c>
       <c r="I28" t="n">
         <v>0.0</v>
@@ -4182,28 +4182,28 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>104</v>
       </c>
       <c r="C29" t="s">
         <v>96</v>
       </c>
       <c r="D29" t="n">
-        <v>46.0</v>
+        <v>35.0</v>
       </c>
       <c r="E29" t="n">
         <v>28.0</v>
       </c>
       <c r="F29" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.0468463097466241</v>
       </c>
       <c r="G29" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H29" t="n">
-        <v>0.0142728080658903</v>
+        <v>0.0417860943528127</v>
       </c>
       <c r="I29" t="n">
         <v>0.0</v>
@@ -4226,28 +4226,28 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C30" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="D30" t="n">
-        <v>35.0</v>
+        <v>28.0</v>
       </c>
       <c r="E30" t="n">
-        <v>28.0</v>
+        <v>25.0</v>
       </c>
       <c r="F30" t="n">
-        <v>0.0468463097466241</v>
+        <v>0.0277777777777778</v>
       </c>
       <c r="G30" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H30" t="n">
-        <v>0.0417860943528127</v>
+        <v>0.00528885616238524</v>
       </c>
       <c r="I30" t="n">
         <v>0.0</v>
@@ -4256,42 +4256,42 @@
         <v>0.0</v>
       </c>
       <c r="K30" t="n">
-        <v>0.05919661733615222</v>
+        <v>0.052854122621564484</v>
       </c>
       <c r="L30" t="n">
         <v>0.0</v>
       </c>
       <c r="M30" t="n">
-        <v>0.0591966173361522</v>
+        <v>0.0528541226215645</v>
       </c>
       <c r="N30" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C31" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D31" t="n">
-        <v>28.0</v>
+        <v>31.0</v>
       </c>
       <c r="E31" t="n">
         <v>25.0</v>
       </c>
       <c r="F31" t="n">
-        <v>0.0277777777777778</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G31" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0158730158730159</v>
       </c>
       <c r="H31" t="n">
-        <v>0.00528885616238524</v>
+        <v>0.00130554100709877</v>
       </c>
       <c r="I31" t="n">
         <v>0.0</v>
@@ -4303,39 +4303,39 @@
         <v>0.052854122621564484</v>
       </c>
       <c r="L31" t="n">
-        <v>3.271025955591198E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M31" t="n">
         <v>0.0528541226215645</v>
       </c>
       <c r="N31" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B32" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D32" t="n">
-        <v>31.0</v>
+        <v>84.0</v>
       </c>
       <c r="E32" t="n">
-        <v>25.0</v>
+        <v>46.0</v>
       </c>
       <c r="F32" t="n">
         <v>0.0059626167965088</v>
       </c>
       <c r="G32" t="n">
-        <v>0.0158730158730159</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="H32" t="n">
-        <v>0.00130554100709877</v>
+        <v>0.00153994324064719</v>
       </c>
       <c r="I32" t="n">
         <v>0.0</v>
@@ -4344,13 +4344,13 @@
         <v>0.0</v>
       </c>
       <c r="K32" t="n">
-        <v>0.052854122621564484</v>
+        <v>0.09725158562367865</v>
       </c>
       <c r="L32" t="n">
-        <v>3.271025955591198E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M32" t="n">
-        <v>0.0528541226215645</v>
+        <v>0.0972515856236787</v>
       </c>
       <c r="N32" t="n">
         <v>0.0</v>
@@ -4358,28 +4358,28 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="C33" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="D33" t="n">
-        <v>84.0</v>
+        <v>31.0</v>
       </c>
       <c r="E33" t="n">
-        <v>46.0</v>
+        <v>25.0</v>
       </c>
       <c r="F33" t="n">
+        <v>0.0172268185197356</v>
+      </c>
+      <c r="G33" t="n">
         <v>0.0059626167965088</v>
       </c>
-      <c r="G33" t="n">
-        <v>0.00396825396825397</v>
-      </c>
       <c r="H33" t="n">
-        <v>0.00153994324064719</v>
+        <v>0.00352256830938948</v>
       </c>
       <c r="I33" t="n">
         <v>0.0</v>
@@ -4388,16 +4388,16 @@
         <v>0.0</v>
       </c>
       <c r="K33" t="n">
-        <v>0.09725158562367865</v>
+        <v>0.052854122621564484</v>
       </c>
       <c r="L33" t="n">
         <v>0.0</v>
       </c>
       <c r="M33" t="n">
-        <v>0.0972515856236787</v>
+        <v>0.0528541226215645</v>
       </c>
       <c r="N33" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="34">
@@ -4405,31 +4405,31 @@
         <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="C34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D34" t="n">
-        <v>31.0</v>
+        <v>250.0</v>
       </c>
       <c r="E34" t="n">
         <v>25.0</v>
       </c>
       <c r="F34" t="n">
-        <v>0.0172268185197356</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G34" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="H34" t="n">
-        <v>0.00352256830938948</v>
+        <v>0.00148405904181779</v>
       </c>
       <c r="I34" t="n">
         <v>0.0</v>
       </c>
       <c r="J34" t="n">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
       <c r="K34" t="n">
         <v>0.052854122621564484</v>
@@ -4441,77 +4441,77 @@
         <v>0.0528541226215645</v>
       </c>
       <c r="N34" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C35" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="D35" t="n">
-        <v>250.0</v>
+        <v>93.0</v>
       </c>
       <c r="E35" t="n">
-        <v>25.0</v>
+        <v>31.0</v>
       </c>
       <c r="F35" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0058336561716597</v>
       </c>
       <c r="G35" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H35" t="n">
-        <v>0.00148405904181779</v>
+        <v>0.0572545435376393</v>
       </c>
       <c r="I35" t="n">
         <v>0.0</v>
       </c>
       <c r="J35" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="K35" t="n">
-        <v>0.052854122621564484</v>
+        <v>0.06553911205073996</v>
       </c>
       <c r="L35" t="n">
-        <v>0.0</v>
+        <v>4.625929269271485E-18</v>
       </c>
       <c r="M35" t="n">
-        <v>0.0528541226215645</v>
+        <v>0.06553911205074</v>
       </c>
       <c r="N35" t="n">
-        <v>0.0</v>
+        <v>4.62592926927149E-18</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C36" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="D36" t="n">
-        <v>93.0</v>
+        <v>250.0</v>
       </c>
       <c r="E36" t="n">
-        <v>31.0</v>
+        <v>64.0</v>
       </c>
       <c r="F36" t="n">
-        <v>0.0058336561716597</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G36" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H36" t="n">
-        <v>0.0572545435376393</v>
+        <v>0.0500405705476867</v>
       </c>
       <c r="I36" t="n">
         <v>0.0</v>
@@ -4520,13 +4520,13 @@
         <v>0.0</v>
       </c>
       <c r="K36" t="n">
-        <v>0.06553911205073996</v>
+        <v>0.13530655391120508</v>
       </c>
       <c r="L36" t="n">
         <v>0.0</v>
       </c>
       <c r="M36" t="n">
-        <v>0.06553911205074</v>
+        <v>0.135306553911205</v>
       </c>
       <c r="N36" t="n">
         <v>0.0</v>
@@ -4534,28 +4534,28 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="C37" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="D37" t="n">
-        <v>250.0</v>
+        <v>37.0</v>
       </c>
       <c r="E37" t="n">
-        <v>64.0</v>
+        <v>27.0</v>
       </c>
       <c r="F37" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.00798534817689006</v>
       </c>
       <c r="G37" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H37" t="n">
-        <v>0.0500405705476867</v>
+        <v>0.00573068158794917</v>
       </c>
       <c r="I37" t="n">
         <v>0.0</v>
@@ -4564,13 +4564,13 @@
         <v>0.0</v>
       </c>
       <c r="K37" t="n">
-        <v>0.13530655391120508</v>
+        <v>0.05708245243128964</v>
       </c>
       <c r="L37" t="n">
         <v>0.0</v>
       </c>
       <c r="M37" t="n">
-        <v>0.135306553911205</v>
+        <v>0.0570824524312896</v>
       </c>
       <c r="N37" t="n">
         <v>0.0</v>
@@ -4578,28 +4578,28 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B38" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C38" t="s">
         <v>102</v>
       </c>
       <c r="D38" t="n">
-        <v>37.0</v>
+        <v>41.0</v>
       </c>
       <c r="E38" t="n">
         <v>27.0</v>
       </c>
       <c r="F38" t="n">
-        <v>0.00798534817689006</v>
+        <v>0.00793650793650794</v>
       </c>
       <c r="G38" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H38" t="n">
-        <v>0.00573068158794917</v>
+        <v>0.00496140462033587</v>
       </c>
       <c r="I38" t="n">
         <v>0.0</v>
@@ -4622,28 +4622,28 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B39" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C39" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="D39" t="n">
-        <v>41.0</v>
+        <v>59.0</v>
       </c>
       <c r="E39" t="n">
-        <v>27.0</v>
+        <v>31.0</v>
       </c>
       <c r="F39" t="n">
-        <v>0.00793650793650794</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G39" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H39" t="n">
-        <v>0.00496140462033587</v>
+        <v>0.00872783618701037</v>
       </c>
       <c r="I39" t="n">
         <v>0.0</v>
@@ -4652,13 +4652,13 @@
         <v>0.0</v>
       </c>
       <c r="K39" t="n">
-        <v>0.05708245243128964</v>
+        <v>0.06553911205073996</v>
       </c>
       <c r="L39" t="n">
-        <v>0.0</v>
+        <v>4.625929269271485E-18</v>
       </c>
       <c r="M39" t="n">
-        <v>0.0570824524312896</v>
+        <v>0.06553911205074</v>
       </c>
       <c r="N39" t="n">
         <v>0.0</v>
@@ -4666,16 +4666,16 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B40" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="C40" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D40" t="n">
-        <v>59.0</v>
+        <v>78.0</v>
       </c>
       <c r="E40" t="n">
         <v>31.0</v>
@@ -4687,7 +4687,7 @@
         <v>0.00396825396825397</v>
       </c>
       <c r="H40" t="n">
-        <v>0.00872783618701037</v>
+        <v>0.0865916560787768</v>
       </c>
       <c r="I40" t="n">
         <v>0.0</v>
@@ -4710,28 +4710,28 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B41" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C41" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="D41" t="n">
-        <v>78.0</v>
+        <v>222.0</v>
       </c>
       <c r="E41" t="n">
-        <v>31.0</v>
+        <v>37.0</v>
       </c>
       <c r="F41" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G41" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H41" t="n">
-        <v>0.0865916560787768</v>
+        <v>0.00201437246540173</v>
       </c>
       <c r="I41" t="n">
         <v>0.0</v>
@@ -4740,42 +4740,42 @@
         <v>0.0</v>
       </c>
       <c r="K41" t="n">
-        <v>0.06553911205073996</v>
+        <v>0.07822410147991543</v>
       </c>
       <c r="L41" t="n">
-        <v>4.625929269271485E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M41" t="n">
-        <v>0.06553911205074</v>
+        <v>0.0782241014799154</v>
       </c>
       <c r="N41" t="n">
-        <v>6.5420519111824E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B42" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="C42" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="D42" t="n">
-        <v>222.0</v>
+        <v>46.0</v>
       </c>
       <c r="E42" t="n">
-        <v>37.0</v>
+        <v>23.0</v>
       </c>
       <c r="F42" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0059626167965088</v>
       </c>
       <c r="G42" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H42" t="n">
-        <v>0.00201437246540173</v>
+        <v>0.145038385111565</v>
       </c>
       <c r="I42" t="n">
         <v>0.0</v>
@@ -4784,13 +4784,13 @@
         <v>0.0</v>
       </c>
       <c r="K42" t="n">
-        <v>0.07822410147991543</v>
+        <v>0.048625792811839326</v>
       </c>
       <c r="L42" t="n">
         <v>0.0</v>
       </c>
       <c r="M42" t="n">
-        <v>0.0782241014799154</v>
+        <v>0.0486257928118393</v>
       </c>
       <c r="N42" t="n">
         <v>0.0</v>
@@ -4798,16 +4798,16 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B43" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C43" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D43" t="n">
-        <v>46.0</v>
+        <v>93.0</v>
       </c>
       <c r="E43" t="n">
         <v>23.0</v>
@@ -4816,10 +4816,10 @@
         <v>0.0059626167965088</v>
       </c>
       <c r="G43" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0158730158730159</v>
       </c>
       <c r="H43" t="n">
-        <v>0.145038385111565</v>
+        <v>0.0914870429913643</v>
       </c>
       <c r="I43" t="n">
         <v>0.0</v>
@@ -4831,7 +4831,7 @@
         <v>0.048625792811839326</v>
       </c>
       <c r="L43" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M43" t="n">
         <v>0.0486257928118393</v>
@@ -4842,40 +4842,40 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B44" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D44" t="n">
-        <v>93.0</v>
+        <v>265.0</v>
       </c>
       <c r="E44" t="n">
         <v>23.0</v>
       </c>
       <c r="F44" t="n">
-        <v>0.0059626167965088</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="G44" t="n">
-        <v>0.0158730158730159</v>
+        <v>0.00396825396825397</v>
       </c>
       <c r="H44" t="n">
-        <v>0.0914870429913643</v>
+        <v>9.13202144083936E-5</v>
       </c>
       <c r="I44" t="n">
         <v>0.0</v>
       </c>
       <c r="J44" t="n">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
       <c r="K44" t="n">
         <v>0.048625792811839326</v>
       </c>
       <c r="L44" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M44" t="n">
         <v>0.0486257928118393</v>
@@ -4886,43 +4886,43 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B45" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C45" t="s">
         <v>92</v>
       </c>
       <c r="D45" t="n">
-        <v>265.0</v>
+        <v>26.0</v>
       </c>
       <c r="E45" t="n">
-        <v>23.0</v>
+        <v>26.0</v>
       </c>
       <c r="F45" t="n">
-        <v>0.00396825396825397</v>
+        <v>0.0166693416357932</v>
       </c>
       <c r="G45" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H45" t="n">
-        <v>9.13202144083936E-5</v>
+        <v>0.0165947985726984</v>
       </c>
       <c r="I45" t="n">
         <v>0.0</v>
       </c>
       <c r="J45" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="K45" t="n">
-        <v>0.048625792811839326</v>
+        <v>0.05496828752642706</v>
       </c>
       <c r="L45" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M45" t="n">
-        <v>0.0486257928118393</v>
+        <v>0.0549682875264271</v>
       </c>
       <c r="N45" t="n">
         <v>2.31296463463574E-18</v>
@@ -4930,34 +4930,34 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C46" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D46" t="n">
-        <v>26.0</v>
+        <v>25.0</v>
       </c>
       <c r="E46" t="n">
         <v>26.0</v>
       </c>
       <c r="F46" t="n">
-        <v>0.0166693416357932</v>
+        <v>0.414406187123225</v>
       </c>
       <c r="G46" t="n">
         <v>0.00396825396825397</v>
       </c>
       <c r="H46" t="n">
-        <v>0.0165947985726984</v>
+        <v>0.00877923124276454</v>
       </c>
       <c r="I46" t="n">
         <v>0.0</v>
       </c>
       <c r="J46" t="n">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
       <c r="K46" t="n">
         <v>0.05496828752642706</v>
@@ -4966,10 +4966,10 @@
         <v>0.0</v>
       </c>
       <c r="M46" t="n">
-        <v>0.0549682875264271</v>
+        <v>0.0551797040169133</v>
       </c>
       <c r="N46" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>6.68557644855895E-4</v>
       </c>
     </row>
     <row r="47">
@@ -4977,10 +4977,10 @@
         <v>64</v>
       </c>
       <c r="B47" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C47" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D47" t="n">
         <v>250.0</v>
@@ -5068,7 +5068,7 @@
         <v>78</v>
       </c>
       <c r="C49" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D49" t="n">
         <v>93.0</v>
@@ -5109,10 +5109,10 @@
         <v>133</v>
       </c>
       <c r="B50" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C50" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D50" t="n">
         <v>250.0</v>
@@ -5145,7 +5145,7 @@
         <v>0.101479915433404</v>
       </c>
       <c r="N50" t="n">
-        <v>4.62592926927149E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="51">
@@ -5153,10 +5153,10 @@
         <v>134</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C51" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D51" t="n">
         <v>250.0</v>
@@ -5197,7 +5197,7 @@
         <v>135</v>
       </c>
       <c r="B52" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C52" t="s">
         <v>107</v>
@@ -5241,7 +5241,7 @@
         <v>136</v>
       </c>
       <c r="B53" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C53" t="s">
         <v>75</v>
@@ -5326,13 +5326,13 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B55" t="s">
         <v>80</v>
       </c>
       <c r="C55" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D55" t="e">
         <v>#NUM!</v>
@@ -5359,7 +5359,7 @@
         <v>0.0613107822410148</v>
       </c>
       <c r="L55" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M55" t="e">
         <v>#NUM!</v>
@@ -5370,7 +5370,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B56" t="s">
         <v>80</v>
@@ -5464,7 +5464,7 @@
         <v>80</v>
       </c>
       <c r="C58" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D58" t="e">
         <v>#NUM!</v>
@@ -5546,7 +5546,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B60" t="s">
         <v>80</v>
@@ -5596,7 +5596,7 @@
         <v>80</v>
       </c>
       <c r="C61" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D61" t="e">
         <v>#NUM!</v>
@@ -5684,7 +5684,7 @@
         <v>80</v>
       </c>
       <c r="C63" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D63" t="e">
         <v>#NUM!</v>
@@ -5884,10 +5884,10 @@
         <v>#NUM!</v>
       </c>
       <c r="K67" t="n">
-        <v>0.48710359408033826</v>
+        <v>0.49577167019027485</v>
       </c>
       <c r="L67" t="n">
-        <v>0.009359807027982536</v>
+        <v>0.018863648786926254</v>
       </c>
       <c r="M67" t="e">
         <v>#NUM!</v>

</xml_diff>